<commit_message>
Criar funcionalidade e tela com tabela para mostrar reservas em progresso por cliente e filial e opcionar cancelamento
</commit_message>
<xml_diff>
--- a/doc/Planejamento.xlsx
+++ b/doc/Planejamento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t xml:space="preserve">Planejado</t>
   </si>
@@ -55,49 +55,46 @@
     <t xml:space="preserve">Criar funcionalidade e tela com tabela para mostrar reservas em progresso por cliente e filial e opcionar cancelamento</t>
   </si>
   <si>
+    <t xml:space="preserve">Finalizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar funcionalidade e tela com tabela para vizualização de categorias reservadas com quantidade reservada e disponivel por filial e data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pendente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iniciar locação  não / não aproveitando reserva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalizar locação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 min = 0,25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar veículos disponíveis para locação  por filial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 min = 0,16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar veículos com locação em progresso por pela filial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 min = 0,33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manutenção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar veículos pendentes  </t>
+  </si>
+  <si>
     <t xml:space="preserve">Em Curso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15:10:00  - 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criar funcionalidade e tela com tabela para vizualização de categorias reservadas com quantidade reservada e disponivel por filial e data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iniciar locação  não / não aproveitando reserva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalizar locação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 min = 0,25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listar veículos disponíveis para locação  por filial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalizado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 min = 0,16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listar veículos com locação em progresso por pela filial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 min = 0,33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manutenção</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listar veículos pendentes  </t>
   </si>
   <si>
     <t xml:space="preserve">30 min = 0,50</t>
@@ -329,8 +326,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
@@ -341,8 +338,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -394,7 +391,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -491,6 +488,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -527,20 +528,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -699,8 +700,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -767,7 +768,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="n">
         <f aca="false">SUM(F6:F25)</f>
-        <v>0</v>
+        <v>8.33</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="0"/>
@@ -842,19 +843,19 @@
         <v>2</v>
       </c>
       <c r="E6" s="22"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="21" t="n">
+        <v>8.33</v>
+      </c>
       <c r="G6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
@@ -862,15 +863,15 @@
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="21" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="21"/>
-      <c r="G7" s="25" t="s">
-        <v>14</v>
+      <c r="G7" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
@@ -886,24 +887,24 @@
       <c r="A8" s="18" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>16</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22"/>
       <c r="F8" s="21"/>
-      <c r="G8" s="25" t="s">
-        <v>14</v>
+      <c r="G8" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
       <c r="N8" s="0"/>
       <c r="O8" s="0"/>
       <c r="P8" s="0"/>
@@ -915,24 +916,24 @@
       <c r="A9" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="28" t="s">
-        <v>17</v>
+      <c r="B9" s="27"/>
+      <c r="C9" s="29" t="s">
+        <v>16</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="22"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="29"/>
+      <c r="G9" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="30"/>
       <c r="I9" s="0"/>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
-      <c r="L9" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="30"/>
+      <c r="L9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="31"/>
       <c r="N9" s="8"/>
       <c r="O9" s="0"/>
       <c r="P9" s="0"/>
@@ -944,26 +945,26 @@
       <c r="A10" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="31" t="s">
-        <v>19</v>
+      <c r="B10" s="27"/>
+      <c r="C10" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
       <c r="F10" s="21"/>
-      <c r="G10" s="25" t="s">
-        <v>14</v>
+      <c r="G10" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H10" s="0"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="30"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="31"/>
       <c r="N10" s="0"/>
       <c r="O10" s="0"/>
       <c r="P10" s="0"/>
@@ -975,26 +976,26 @@
       <c r="A11" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="25" t="s">
-        <v>14</v>
+      <c r="G11" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H11" s="0"/>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
       <c r="K11" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="30"/>
+        <v>13</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="31"/>
       <c r="N11" s="0"/>
       <c r="O11" s="36"/>
       <c r="P11" s="36"/>
@@ -1006,28 +1007,28 @@
       <c r="A12" s="18" t="n">
         <v>7</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>24</v>
+      <c r="B12" s="27" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="25" t="s">
-        <v>14</v>
+      <c r="G12" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H12" s="0"/>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
-      <c r="K12" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="30"/>
+      <c r="K12" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="31"/>
       <c r="N12" s="0"/>
       <c r="O12" s="0"/>
       <c r="P12" s="0"/>
@@ -1039,24 +1040,24 @@
       <c r="A13" s="18" t="n">
         <v>8</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="31" t="s">
-        <v>27</v>
+      <c r="B13" s="27"/>
+      <c r="C13" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="25" t="s">
-        <v>14</v>
+      <c r="G13" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
-      <c r="L13" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13" s="30"/>
+      <c r="L13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="31"/>
       <c r="N13" s="0"/>
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
@@ -1065,45 +1066,45 @@
       <c r="A14" s="18" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="31" t="s">
-        <v>29</v>
+      <c r="B14" s="27"/>
+      <c r="C14" s="32" t="s">
+        <v>28</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="25" t="s">
-        <v>14</v>
+      <c r="G14" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
-      <c r="L14" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" s="30"/>
+      <c r="L14" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="n">
         <v>10</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>31</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>32</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="25" t="s">
-        <v>14</v>
+      <c r="G15" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
-      <c r="K15" s="29"/>
+      <c r="K15" s="30"/>
       <c r="L15" s="0"/>
       <c r="M15" s="0"/>
     </row>
@@ -1111,15 +1112,15 @@
       <c r="A16" s="18" t="n">
         <v>11</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="31" t="s">
-        <v>33</v>
+      <c r="B16" s="27"/>
+      <c r="C16" s="32" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="25" t="s">
-        <v>14</v>
+      <c r="G16" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
@@ -1132,9 +1133,9 @@
       <c r="A17" s="18" t="n">
         <v>12</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="38" t="s">
-        <v>34</v>
+      <c r="B17" s="27"/>
+      <c r="C17" s="39" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="22" t="e">
@@ -1142,8 +1143,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="25" t="s">
-        <v>14</v>
+      <c r="G17" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -1156,9 +1157,9 @@
       <c r="A18" s="18" t="n">
         <v>13</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="31" t="s">
-        <v>35</v>
+      <c r="B18" s="27"/>
+      <c r="C18" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="22" t="e">
@@ -1166,8 +1167,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="25" t="s">
-        <v>14</v>
+      <c r="G18" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -1180,9 +1181,9 @@
       <c r="A19" s="18" t="n">
         <v>14</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="31" t="s">
-        <v>36</v>
+      <c r="B19" s="27"/>
+      <c r="C19" s="32" t="s">
+        <v>35</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="22" t="e">
@@ -1190,8 +1191,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F19" s="21"/>
-      <c r="G19" s="25" t="s">
-        <v>14</v>
+      <c r="G19" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -1207,9 +1208,9 @@
       <c r="A20" s="18" t="n">
         <v>15</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="31" t="s">
-        <v>37</v>
+      <c r="B20" s="27"/>
+      <c r="C20" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22" t="e">
@@ -1217,8 +1218,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F20" s="21"/>
-      <c r="G20" s="25" t="s">
-        <v>14</v>
+      <c r="G20" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
@@ -1231,9 +1232,9 @@
       <c r="A21" s="18" t="n">
         <v>16</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="39" t="s">
-        <v>38</v>
+      <c r="B21" s="27"/>
+      <c r="C21" s="40" t="s">
+        <v>37</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="22" t="e">
@@ -1241,8 +1242,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F21" s="21"/>
-      <c r="G21" s="25" t="s">
-        <v>14</v>
+      <c r="G21" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
@@ -1258,9 +1259,9 @@
       <c r="A22" s="18" t="n">
         <v>17</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="31" t="s">
-        <v>39</v>
+      <c r="B22" s="27"/>
+      <c r="C22" s="32" t="s">
+        <v>38</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="22" t="e">
@@ -1268,8 +1269,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F22" s="21"/>
-      <c r="G22" s="25" t="s">
-        <v>14</v>
+      <c r="G22" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
@@ -1285,15 +1286,15 @@
       <c r="A23" s="18" t="n">
         <v>18</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="40" t="s">
-        <v>40</v>
+      <c r="B23" s="27"/>
+      <c r="C23" s="41" t="s">
+        <v>39</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="25" t="s">
-        <v>14</v>
+      <c r="G23" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
@@ -1306,9 +1307,9 @@
       <c r="A24" s="18" t="n">
         <v>19</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="40" t="s">
-        <v>41</v>
+      <c r="B24" s="27"/>
+      <c r="C24" s="41" t="s">
+        <v>40</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="22" t="e">
@@ -1316,8 +1317,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F24" s="21"/>
-      <c r="G24" s="25" t="s">
-        <v>14</v>
+      <c r="G24" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
@@ -1330,9 +1331,9 @@
       <c r="A25" s="18" t="n">
         <v>20</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="40" t="s">
-        <v>42</v>
+      <c r="B25" s="27"/>
+      <c r="C25" s="41" t="s">
+        <v>41</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="22" t="e">
@@ -1340,8 +1341,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F25" s="21"/>
-      <c r="G25" s="25" t="s">
-        <v>14</v>
+      <c r="G25" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
@@ -1355,17 +1356,17 @@
     </row>
     <row r="26" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="41" t="s">
         <v>43</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>44</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
       <c r="F26" s="21"/>
-      <c r="G26" s="25" t="s">
-        <v>14</v>
+      <c r="G26" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H26" s="0"/>
       <c r="I26" s="0"/>
@@ -1379,15 +1380,15 @@
     </row>
     <row r="27" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="40" t="s">
-        <v>45</v>
+      <c r="B27" s="27"/>
+      <c r="C27" s="41" t="s">
+        <v>44</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="21"/>
-      <c r="G27" s="25" t="s">
-        <v>14</v>
+      <c r="G27" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
@@ -1401,17 +1402,17 @@
     </row>
     <row r="28" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="41" t="s">
         <v>46</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>47</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="21"/>
-      <c r="G28" s="25" t="s">
-        <v>14</v>
+      <c r="G28" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H28" s="0"/>
       <c r="I28" s="0"/>
@@ -1425,15 +1426,15 @@
     </row>
     <row r="29" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="40" t="s">
-        <v>48</v>
+      <c r="B29" s="27"/>
+      <c r="C29" s="41" t="s">
+        <v>47</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
       <c r="F29" s="21"/>
-      <c r="G29" s="25" t="s">
-        <v>14</v>
+      <c r="G29" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H29" s="0"/>
       <c r="I29" s="0"/>
@@ -1447,15 +1448,15 @@
     </row>
     <row r="30" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="40" t="s">
-        <v>49</v>
+      <c r="B30" s="27"/>
+      <c r="C30" s="41" t="s">
+        <v>48</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
       <c r="F30" s="21"/>
-      <c r="G30" s="25" t="s">
-        <v>14</v>
+      <c r="G30" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H30" s="0"/>
       <c r="I30" s="0"/>
@@ -1469,15 +1470,15 @@
     </row>
     <row r="31" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="41" t="s">
-        <v>50</v>
+      <c r="B31" s="27"/>
+      <c r="C31" s="42" t="s">
+        <v>49</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
       <c r="F31" s="21"/>
-      <c r="G31" s="25" t="s">
-        <v>14</v>
+      <c r="G31" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
@@ -1491,17 +1492,17 @@
     </row>
     <row r="32" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="41" t="s">
         <v>51</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>52</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
       <c r="F32" s="21"/>
-      <c r="G32" s="25" t="s">
-        <v>14</v>
+      <c r="G32" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H32" s="0"/>
       <c r="I32" s="0"/>
@@ -1515,15 +1516,15 @@
     </row>
     <row r="33" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="40" t="s">
-        <v>53</v>
+      <c r="B33" s="27"/>
+      <c r="C33" s="41" t="s">
+        <v>52</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
       <c r="F33" s="21"/>
-      <c r="G33" s="25" t="s">
-        <v>14</v>
+      <c r="G33" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
@@ -1537,17 +1538,17 @@
     </row>
     <row r="34" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="43" t="s">
         <v>54</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>55</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
       <c r="F34" s="21"/>
-      <c r="G34" s="25" t="s">
-        <v>14</v>
+      <c r="G34" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H34" s="0"/>
       <c r="I34" s="0"/>
@@ -1561,17 +1562,17 @@
     </row>
     <row r="35" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="45" t="s">
         <v>56</v>
-      </c>
-      <c r="C35" s="44" t="s">
-        <v>57</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="21"/>
-      <c r="G35" s="25" t="s">
-        <v>14</v>
+      <c r="G35" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
@@ -1585,17 +1586,17 @@
     </row>
     <row r="36" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="41" t="s">
         <v>58</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>59</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="21"/>
-      <c r="G36" s="25" t="s">
-        <v>14</v>
+      <c r="G36" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H36" s="0"/>
       <c r="I36" s="0"/>
@@ -1609,15 +1610,15 @@
     </row>
     <row r="37" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="40" t="s">
-        <v>60</v>
+      <c r="B37" s="27"/>
+      <c r="C37" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
       <c r="F37" s="21"/>
-      <c r="G37" s="25" t="s">
-        <v>14</v>
+      <c r="G37" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="H37" s="0"/>
       <c r="I37" s="0"/>
@@ -1629,8 +1630,8 @@
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" s="46" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="45"/>
+    <row r="38" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="46"/>
       <c r="B38" s="0"/>
       <c r="C38" s="0"/>
       <c r="D38" s="0"/>
@@ -1647,8 +1648,8 @@
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" s="46" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="45"/>
+    <row r="39" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="46"/>
       <c r="B39" s="0"/>
       <c r="C39" s="0"/>
       <c r="D39" s="0"/>
@@ -1665,8 +1666,8 @@
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" s="46" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="45"/>
+    <row r="40" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="46"/>
       <c r="B40" s="0"/>
       <c r="C40" s="0"/>
       <c r="D40" s="0"/>
@@ -1683,8 +1684,8 @@
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
-    <row r="41" s="46" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="45"/>
+    <row r="41" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="46"/>
       <c r="B41" s="0"/>
       <c r="C41" s="0"/>
       <c r="D41" s="0"/>
@@ -1701,8 +1702,8 @@
       <c r="AMI41" s="0"/>
       <c r="AMJ41" s="0"/>
     </row>
-    <row r="42" s="46" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="45"/>
+    <row r="42" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="46"/>
       <c r="B42" s="0"/>
       <c r="C42" s="0"/>
       <c r="D42" s="0"/>
@@ -1719,8 +1720,8 @@
       <c r="AMI42" s="0"/>
       <c r="AMJ42" s="0"/>
     </row>
-    <row r="43" s="47" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="45"/>
+    <row r="43" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="46"/>
       <c r="B43" s="0"/>
       <c r="C43" s="0"/>
       <c r="D43" s="0"/>
@@ -1737,8 +1738,8 @@
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" s="47" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="45"/>
+    <row r="44" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="46"/>
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
       <c r="D44" s="0"/>
@@ -1755,8 +1756,8 @@
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" s="47" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="45"/>
+    <row r="45" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="46"/>
       <c r="B45" s="0"/>
       <c r="C45" s="0"/>
       <c r="D45" s="0"/>
@@ -1773,8 +1774,8 @@
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
-    <row r="46" s="47" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="45"/>
+    <row r="46" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="46"/>
       <c r="B46" s="0"/>
       <c r="C46" s="0"/>
       <c r="D46" s="0"/>
@@ -1791,8 +1792,8 @@
       <c r="AMI46" s="0"/>
       <c r="AMJ46" s="0"/>
     </row>
-    <row r="47" s="47" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="45"/>
+    <row r="47" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="46"/>
       <c r="B47" s="0"/>
       <c r="C47" s="0"/>
       <c r="D47" s="0"/>
@@ -1810,7 +1811,7 @@
       <c r="AMJ47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="45"/>
+      <c r="A48" s="46"/>
       <c r="C48" s="0"/>
       <c r="G48" s="0"/>
       <c r="H48" s="0"/>
@@ -1821,7 +1822,7 @@
       <c r="M48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="45"/>
+      <c r="A49" s="46"/>
       <c r="C49" s="0"/>
       <c r="G49" s="0"/>
       <c r="H49" s="0"/>
@@ -1832,7 +1833,7 @@
       <c r="M49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="45"/>
+      <c r="A50" s="46"/>
       <c r="C50" s="0"/>
       <c r="G50" s="0"/>
       <c r="H50" s="0"/>
@@ -1843,7 +1844,7 @@
       <c r="M50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="45"/>
+      <c r="A51" s="46"/>
       <c r="C51" s="0"/>
       <c r="G51" s="0"/>
       <c r="H51" s="0"/>
@@ -1854,7 +1855,7 @@
       <c r="M51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="45"/>
+      <c r="A52" s="46"/>
       <c r="C52" s="0"/>
       <c r="G52" s="0"/>
       <c r="H52" s="0"/>
@@ -1865,7 +1866,7 @@
       <c r="M52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="45"/>
+      <c r="A53" s="46"/>
       <c r="C53" s="0"/>
       <c r="G53" s="0"/>
       <c r="H53" s="0"/>
@@ -1876,7 +1877,7 @@
       <c r="M53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="45"/>
+      <c r="A54" s="46"/>
       <c r="C54" s="0"/>
       <c r="G54" s="0"/>
       <c r="H54" s="0"/>
@@ -1887,7 +1888,7 @@
       <c r="M54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="45"/>
+      <c r="A55" s="46"/>
       <c r="C55" s="0"/>
       <c r="G55" s="0"/>
       <c r="H55" s="0"/>
@@ -1898,7 +1899,7 @@
       <c r="M55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="45"/>
+      <c r="A56" s="46"/>
       <c r="C56" s="0"/>
       <c r="G56" s="0"/>
       <c r="H56" s="0"/>
@@ -1909,7 +1910,7 @@
       <c r="M56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="45"/>
+      <c r="A57" s="46"/>
       <c r="C57" s="0"/>
       <c r="G57" s="0"/>
       <c r="H57" s="0"/>
@@ -1920,7 +1921,7 @@
       <c r="M57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="45"/>
+      <c r="A58" s="46"/>
       <c r="C58" s="0"/>
       <c r="G58" s="0"/>
       <c r="H58" s="0"/>
@@ -1931,7 +1932,7 @@
       <c r="M58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="45"/>
+      <c r="A59" s="46"/>
       <c r="C59" s="0"/>
       <c r="G59" s="0"/>
       <c r="H59" s="0"/>
@@ -1942,7 +1943,7 @@
       <c r="M59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="45"/>
+      <c r="A60" s="46"/>
       <c r="C60" s="0"/>
       <c r="G60" s="0"/>
       <c r="H60" s="0"/>
@@ -1953,7 +1954,7 @@
       <c r="M60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="45"/>
+      <c r="A61" s="46"/>
       <c r="C61" s="0"/>
       <c r="G61" s="0"/>
       <c r="H61" s="0"/>
@@ -1964,7 +1965,7 @@
       <c r="M61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="45"/>
+      <c r="A62" s="46"/>
       <c r="C62" s="0"/>
       <c r="G62" s="0"/>
       <c r="H62" s="0"/>
@@ -1975,7 +1976,7 @@
       <c r="M62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="45"/>
+      <c r="A63" s="46"/>
       <c r="C63" s="0"/>
       <c r="G63" s="0"/>
       <c r="H63" s="0"/>
@@ -1986,7 +1987,7 @@
       <c r="M63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="45"/>
+      <c r="A64" s="46"/>
       <c r="C64" s="0"/>
       <c r="G64" s="0"/>
       <c r="H64" s="0"/>
@@ -1997,7 +1998,7 @@
       <c r="M64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="45"/>
+      <c r="A65" s="46"/>
       <c r="C65" s="0"/>
       <c r="G65" s="0"/>
       <c r="H65" s="0"/>
@@ -2008,7 +2009,7 @@
       <c r="M65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="45"/>
+      <c r="A66" s="46"/>
       <c r="C66" s="0"/>
       <c r="G66" s="0"/>
       <c r="H66" s="0"/>
@@ -2019,7 +2020,7 @@
       <c r="M66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="45"/>
+      <c r="A67" s="46"/>
       <c r="C67" s="0"/>
       <c r="G67" s="0"/>
       <c r="H67" s="0"/>
@@ -2030,7 +2031,7 @@
       <c r="M67" s="0"/>
     </row>
     <row r="68" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="45"/>
+      <c r="A68" s="46"/>
       <c r="B68" s="0"/>
       <c r="C68" s="0"/>
       <c r="D68" s="0"/>
@@ -2048,7 +2049,7 @@
       <c r="AMJ68" s="0"/>
     </row>
     <row r="69" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="45"/>
+      <c r="A69" s="46"/>
       <c r="B69" s="0"/>
       <c r="C69" s="0"/>
       <c r="D69" s="0"/>
@@ -2066,7 +2067,7 @@
       <c r="AMJ69" s="0"/>
     </row>
     <row r="70" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="45"/>
+      <c r="A70" s="46"/>
       <c r="B70" s="0"/>
       <c r="C70" s="0"/>
       <c r="D70" s="0"/>
@@ -2084,7 +2085,7 @@
       <c r="AMJ70" s="0"/>
     </row>
     <row r="71" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="45"/>
+      <c r="A71" s="46"/>
       <c r="B71" s="0"/>
       <c r="C71" s="0"/>
       <c r="D71" s="0"/>
@@ -2102,7 +2103,7 @@
       <c r="AMJ71" s="0"/>
     </row>
     <row r="72" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="45"/>
+      <c r="A72" s="46"/>
       <c r="B72" s="0"/>
       <c r="C72" s="0"/>
       <c r="D72" s="0"/>
@@ -2120,7 +2121,7 @@
       <c r="AMJ72" s="0"/>
     </row>
     <row r="73" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="45"/>
+      <c r="A73" s="46"/>
       <c r="B73" s="0"/>
       <c r="C73" s="0"/>
       <c r="D73" s="0"/>
@@ -2138,7 +2139,7 @@
       <c r="AMJ73" s="0"/>
     </row>
     <row r="74" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="45"/>
+      <c r="A74" s="46"/>
       <c r="B74" s="0"/>
       <c r="C74" s="0"/>
       <c r="D74" s="0"/>
@@ -2156,7 +2157,7 @@
       <c r="AMJ74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="45"/>
+      <c r="A75" s="46"/>
       <c r="C75" s="0"/>
       <c r="G75" s="0"/>
       <c r="H75" s="0"/>
@@ -2167,7 +2168,7 @@
       <c r="M75" s="0"/>
     </row>
     <row r="76" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="45"/>
+      <c r="A76" s="46"/>
       <c r="B76" s="0"/>
       <c r="C76" s="0"/>
       <c r="D76" s="0"/>
@@ -2185,7 +2186,7 @@
       <c r="AMJ76" s="0"/>
     </row>
     <row r="77" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="47"/>
+      <c r="A77" s="48"/>
       <c r="B77" s="0"/>
       <c r="C77" s="0"/>
       <c r="D77" s="0"/>
@@ -2203,7 +2204,7 @@
       <c r="AMJ77" s="0"/>
     </row>
     <row r="78" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="47"/>
+      <c r="A78" s="48"/>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
@@ -2221,7 +2222,7 @@
       <c r="AMJ78" s="0"/>
     </row>
     <row r="79" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="47"/>
+      <c r="A79" s="48"/>
       <c r="B79" s="0"/>
       <c r="C79" s="0"/>
       <c r="D79" s="0"/>
@@ -2239,7 +2240,7 @@
       <c r="AMJ79" s="0"/>
     </row>
     <row r="80" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="47"/>
+      <c r="A80" s="48"/>
       <c r="B80" s="0"/>
       <c r="C80" s="0"/>
       <c r="D80" s="0"/>
@@ -2257,7 +2258,7 @@
       <c r="AMJ80" s="0"/>
     </row>
     <row r="81" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="47"/>
+      <c r="A81" s="48"/>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
       <c r="D81" s="0"/>
@@ -2275,7 +2276,7 @@
       <c r="AMJ81" s="0"/>
     </row>
     <row r="82" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="47"/>
+      <c r="A82" s="48"/>
       <c r="B82" s="0"/>
       <c r="C82" s="0"/>
       <c r="D82" s="0"/>
@@ -2293,7 +2294,7 @@
       <c r="AMJ82" s="0"/>
     </row>
     <row r="83" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="47"/>
+      <c r="A83" s="48"/>
       <c r="B83" s="0"/>
       <c r="C83" s="0"/>
       <c r="D83" s="0"/>
@@ -2311,7 +2312,7 @@
       <c r="AMJ83" s="0"/>
     </row>
     <row r="84" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="47"/>
+      <c r="A84" s="48"/>
       <c r="B84" s="0"/>
       <c r="C84" s="0"/>
       <c r="D84" s="0"/>
@@ -2329,7 +2330,7 @@
       <c r="AMJ84" s="0"/>
     </row>
     <row r="85" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="47"/>
+      <c r="A85" s="48"/>
       <c r="B85" s="0"/>
       <c r="C85" s="0"/>
       <c r="D85" s="0"/>
@@ -2347,7 +2348,7 @@
       <c r="AMJ85" s="0"/>
     </row>
     <row r="86" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="47"/>
+      <c r="A86" s="48"/>
       <c r="B86" s="0"/>
       <c r="C86" s="0"/>
       <c r="D86" s="0"/>
@@ -2365,7 +2366,7 @@
       <c r="AMJ86" s="0"/>
     </row>
     <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="47"/>
+      <c r="A87" s="48"/>
       <c r="C87" s="0"/>
       <c r="G87" s="0"/>
       <c r="H87" s="0"/>
@@ -2376,7 +2377,7 @@
       <c r="M87" s="0"/>
     </row>
     <row r="88" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="47"/>
+      <c r="A88" s="48"/>
       <c r="B88" s="0"/>
       <c r="C88" s="0"/>
       <c r="D88" s="0"/>
@@ -2394,7 +2395,7 @@
       <c r="AMJ88" s="0"/>
     </row>
     <row r="89" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="47"/>
+      <c r="A89" s="48"/>
       <c r="B89" s="0"/>
       <c r="C89" s="0"/>
       <c r="D89" s="0"/>
@@ -2412,7 +2413,7 @@
       <c r="AMJ89" s="0"/>
     </row>
     <row r="90" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="47"/>
+      <c r="A90" s="48"/>
       <c r="B90" s="0"/>
       <c r="C90" s="0"/>
       <c r="D90" s="0"/>
@@ -2430,7 +2431,7 @@
       <c r="AMJ90" s="0"/>
     </row>
     <row r="91" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="47"/>
+      <c r="A91" s="48"/>
       <c r="B91" s="0"/>
       <c r="C91" s="0"/>
       <c r="D91" s="0"/>
@@ -2448,7 +2449,7 @@
       <c r="AMJ91" s="0"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="47"/>
+      <c r="A92" s="48"/>
       <c r="C92" s="0"/>
       <c r="G92" s="0"/>
       <c r="H92" s="0"/>
@@ -2459,7 +2460,7 @@
       <c r="M92" s="0"/>
     </row>
     <row r="93" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="47"/>
+      <c r="A93" s="48"/>
       <c r="B93" s="0"/>
       <c r="C93" s="0"/>
       <c r="D93" s="0"/>
@@ -3171,13 +3172,12 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="18">
     <mergeCell ref="B1:N1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="H6:N6"/>
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="L10:M10"/>

</xml_diff>

<commit_message>
Buscar categorias de veiculo superiores ; Criar funcionalidade e tela com tabela para vizualização de categorias reservadas com quantidade reservada e disponivel por filial e data
</commit_message>
<xml_diff>
--- a/doc/Planejamento.xlsx
+++ b/doc/Planejamento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t xml:space="preserve">Planejado</t>
   </si>
@@ -61,13 +61,16 @@
     <t xml:space="preserve">Criar funcionalidade e tela com tabela para vizualização de categorias reservadas com quantidade reservada e disponivel por filial e data</t>
   </si>
   <si>
+    <t xml:space="preserve">Locação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar categorias de veiculo superiores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iniciar locação  não / não aproveitando reserva</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pendente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iniciar locação  não / não aproveitando reserva</t>
   </si>
   <si>
     <t xml:space="preserve">Finalizar locação</t>
@@ -484,7 +487,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -500,47 +503,47 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -701,7 +704,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -762,13 +765,13 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="10" t="n">
-        <f aca="false">SUM(D6:D25)</f>
-        <v>4</v>
+        <f aca="false">SUM(D6:D26)</f>
+        <v>7</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="n">
-        <f aca="false">SUM(F6:F25)</f>
-        <v>8.33</v>
+        <f aca="false">SUM(F6:F26)</f>
+        <v>14.99</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="0"/>
@@ -859,292 +862,296 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="2" customFormat="true" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" s="2" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="22"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
-      <c r="L7" s="0"/>
-      <c r="M7" s="0"/>
+      <c r="F7" s="21" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
       <c r="N7" s="0"/>
       <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
-    <row r="8" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" s="27" t="s">
+    <row r="8" s="2" customFormat="true" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="21"/>
+      <c r="D8" s="21" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" s="22"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="0"/>
-      <c r="I8" s="0"/>
-      <c r="J8" s="0"/>
-      <c r="K8" s="0"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="0"/>
-      <c r="O8" s="0"/>
-      <c r="P8" s="0"/>
-      <c r="Q8" s="0"/>
+      <c r="F8" s="21" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="29" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="22"/>
       <c r="F9" s="21"/>
       <c r="G9" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="30"/>
+        <v>16</v>
+      </c>
+      <c r="H9" s="0"/>
       <c r="I9" s="0"/>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
-      <c r="L9" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="31"/>
-      <c r="N9" s="8"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="0"/>
       <c r="O9" s="0"/>
       <c r="P9" s="0"/>
       <c r="Q9" s="0"/>
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="n">
-        <v>5</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="32" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
       <c r="F10" s="21"/>
       <c r="G10" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="0"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="31"/>
-      <c r="N10" s="0"/>
+        <v>16</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="30"/>
+      <c r="N10" s="8"/>
       <c r="O10" s="0"/>
       <c r="P10" s="0"/>
       <c r="Q10" s="0"/>
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="n">
-        <v>6</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="20" t="s">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="31" t="s">
+        <v>19</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="21"/>
       <c r="G11" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H11" s="0"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="30"/>
       <c r="N11" s="0"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
+      <c r="Q11" s="0"/>
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="n">
-        <v>7</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>22</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B12" s="19"/>
       <c r="C12" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
       <c r="F12" s="21"/>
       <c r="G12" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H12" s="0"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="31"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="30"/>
       <c r="N12" s="0"/>
-      <c r="O12" s="0"/>
-      <c r="P12" s="0"/>
-      <c r="Q12" s="0"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="n">
-        <v>8</v>
-      </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="32" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="21"/>
       <c r="G13" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H13" s="0"/>
-      <c r="I13" s="0"/>
-      <c r="J13" s="0"/>
-      <c r="K13" s="0"/>
-      <c r="L13" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="31"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="30"/>
       <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="n">
-        <v>9</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="32" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="31" t="s">
+        <v>27</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="21"/>
       <c r="G14" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="30"/>
+      <c r="N14" s="0"/>
+      <c r="AMI14" s="0"/>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="n">
+        <v>9</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="31" t="s">
         <v>29</v>
-      </c>
-      <c r="M14" s="31"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="n">
-        <v>10</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>31</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="F15" s="21"/>
       <c r="G15" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="0"/>
-      <c r="M15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K15" s="0"/>
+      <c r="L15" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="30"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="n">
-        <v>11</v>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="38" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
       <c r="F16" s="21"/>
       <c r="G16" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
       <c r="J16" s="0"/>
-      <c r="K16" s="0"/>
+      <c r="K16" s="29"/>
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="n">
-        <v>12</v>
-      </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="36"/>
+      <c r="C17" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="21"/>
-      <c r="E17" s="22" t="e">
-        <f aca="false">C18*D17</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="E17" s="22"/>
       <c r="F17" s="21"/>
       <c r="G17" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -1153,12 +1160,12 @@
       <c r="L17" s="0"/>
       <c r="M17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="n">
-        <v>13</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="39" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="21"/>
@@ -1168,7 +1175,7 @@
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -1177,12 +1184,12 @@
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
     </row>
-    <row r="19" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="n">
-        <v>14</v>
-      </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="36"/>
+      <c r="C19" s="31" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="21"/>
@@ -1192,7 +1199,7 @@
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -1200,26 +1207,23 @@
       <c r="K19" s="0"/>
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
-      <c r="N19" s="0"/>
-      <c r="AMI19" s="0"/>
-      <c r="AMJ19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="n">
-        <v>15</v>
-      </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="36"/>
+      <c r="C20" s="31" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22" t="e">
-        <f aca="false">C22*D20</f>
+        <f aca="false">C21*D20</f>
         <v>#VALUE!</v>
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
@@ -1227,23 +1231,26 @@
       <c r="K20" s="0"/>
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
-    </row>
-    <row r="21" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N20" s="0"/>
+      <c r="AMI20" s="0"/>
+      <c r="AMJ20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="n">
-        <v>16</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="36"/>
+      <c r="C21" s="31" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="22" t="e">
-        <f aca="false">C22*D21</f>
+        <f aca="false">C23*D21</f>
         <v>#VALUE!</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
@@ -1251,16 +1258,13 @@
       <c r="K21" s="0"/>
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
-      <c r="N21" s="0"/>
-      <c r="AMI21" s="0"/>
-      <c r="AMJ21" s="0"/>
-    </row>
-    <row r="22" s="2" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="36"/>
+      <c r="C22" s="40" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="21"/>
@@ -1270,7 +1274,7 @@
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
@@ -1282,19 +1286,22 @@
       <c r="AMI22" s="0"/>
       <c r="AMJ22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" s="2" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="n">
-        <v>18</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="31" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
+      <c r="E23" s="22" t="e">
+        <f aca="false">C24*D23</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="F23" s="21"/>
       <c r="G23" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
@@ -1302,23 +1309,23 @@
       <c r="K23" s="0"/>
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N23" s="0"/>
+      <c r="AMI23" s="0"/>
+      <c r="AMJ23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="n">
-        <v>19</v>
-      </c>
-      <c r="B24" s="27"/>
+        <v>18</v>
+      </c>
+      <c r="B24" s="36"/>
       <c r="C24" s="41" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="21"/>
-      <c r="E24" s="22" t="e">
-        <f aca="false">C24*D24</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="E24" s="22"/>
       <c r="F24" s="21"/>
       <c r="G24" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
@@ -1327,11 +1334,11 @@
       <c r="L24" s="0"/>
       <c r="M24" s="0"/>
     </row>
-    <row r="25" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="n">
-        <v>20</v>
-      </c>
-      <c r="B25" s="27"/>
+        <v>19</v>
+      </c>
+      <c r="B25" s="36"/>
       <c r="C25" s="41" t="s">
         <v>41</v>
       </c>
@@ -1342,7 +1349,7 @@
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
@@ -1350,23 +1357,23 @@
       <c r="K25" s="0"/>
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
-      <c r="N25" s="0"/>
-      <c r="AMI25" s="0"/>
-      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18"/>
-      <c r="B26" s="27" t="s">
+      <c r="A26" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>43</v>
-      </c>
       <c r="D26" s="21"/>
-      <c r="E26" s="22"/>
+      <c r="E26" s="22" t="e">
+        <f aca="false">C26*D26</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="F26" s="21"/>
       <c r="G26" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H26" s="0"/>
       <c r="I26" s="0"/>
@@ -1380,7 +1387,9 @@
     </row>
     <row r="27" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
-      <c r="B27" s="27"/>
+      <c r="B27" s="36" t="s">
+        <v>43</v>
+      </c>
       <c r="C27" s="41" t="s">
         <v>44</v>
       </c>
@@ -1388,7 +1397,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="21"/>
       <c r="G27" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
@@ -1402,17 +1411,15 @@
     </row>
     <row r="28" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="36"/>
+      <c r="C28" s="41" t="s">
         <v>45</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>46</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="21"/>
       <c r="G28" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H28" s="0"/>
       <c r="I28" s="0"/>
@@ -1426,7 +1433,9 @@
     </row>
     <row r="29" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
-      <c r="B29" s="27"/>
+      <c r="B29" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="C29" s="41" t="s">
         <v>47</v>
       </c>
@@ -1434,7 +1443,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="21"/>
       <c r="G29" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H29" s="0"/>
       <c r="I29" s="0"/>
@@ -1448,7 +1457,7 @@
     </row>
     <row r="30" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
-      <c r="B30" s="27"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="41" t="s">
         <v>48</v>
       </c>
@@ -1456,7 +1465,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="21"/>
       <c r="G30" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H30" s="0"/>
       <c r="I30" s="0"/>
@@ -1470,15 +1479,15 @@
     </row>
     <row r="31" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="42" t="s">
+      <c r="B31" s="36"/>
+      <c r="C31" s="41" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
       <c r="F31" s="21"/>
       <c r="G31" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
@@ -1492,17 +1501,15 @@
     </row>
     <row r="32" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="36"/>
+      <c r="C32" s="42" t="s">
         <v>50</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>51</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
       <c r="F32" s="21"/>
       <c r="G32" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H32" s="0"/>
       <c r="I32" s="0"/>
@@ -1516,7 +1523,9 @@
     </row>
     <row r="33" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
-      <c r="B33" s="27"/>
+      <c r="B33" s="36" t="s">
+        <v>51</v>
+      </c>
       <c r="C33" s="41" t="s">
         <v>52</v>
       </c>
@@ -1524,7 +1533,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="21"/>
       <c r="G33" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
@@ -1536,19 +1545,17 @@
       <c r="AMI33" s="0"/>
       <c r="AMJ33" s="0"/>
     </row>
-    <row r="34" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="36"/>
+      <c r="C34" s="41" t="s">
         <v>53</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>54</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
       <c r="F34" s="21"/>
       <c r="G34" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H34" s="0"/>
       <c r="I34" s="0"/>
@@ -1562,17 +1569,17 @@
     </row>
     <row r="35" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="43" t="s">
         <v>55</v>
-      </c>
-      <c r="C35" s="45" t="s">
-        <v>56</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="21"/>
       <c r="G35" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
@@ -1586,17 +1593,17 @@
     </row>
     <row r="36" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="45" t="s">
         <v>57</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>58</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="21"/>
       <c r="G36" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H36" s="0"/>
       <c r="I36" s="0"/>
@@ -1610,7 +1617,9 @@
     </row>
     <row r="37" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
-      <c r="B37" s="27"/>
+      <c r="B37" s="36" t="s">
+        <v>58</v>
+      </c>
       <c r="C37" s="41" t="s">
         <v>59</v>
       </c>
@@ -1618,7 +1627,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="21"/>
       <c r="G37" s="26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H37" s="0"/>
       <c r="I37" s="0"/>
@@ -1630,14 +1639,18 @@
       <c r="AMI37" s="0"/>
       <c r="AMJ37" s="0"/>
     </row>
-    <row r="38" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="46"/>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="0"/>
-      <c r="E38" s="0"/>
-      <c r="F38" s="0"/>
-      <c r="G38" s="0"/>
+    <row r="38" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="18"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="21"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="26" t="s">
+        <v>16</v>
+      </c>
       <c r="H38" s="0"/>
       <c r="I38" s="0"/>
       <c r="J38" s="0"/>
@@ -1720,7 +1733,7 @@
       <c r="AMI42" s="0"/>
       <c r="AMJ42" s="0"/>
     </row>
-    <row r="43" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="46"/>
       <c r="B43" s="0"/>
       <c r="C43" s="0"/>
@@ -1810,9 +1823,13 @@
       <c r="AMI47" s="0"/>
       <c r="AMJ47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="46"/>
+      <c r="B48" s="0"/>
       <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
+      <c r="F48" s="0"/>
       <c r="G48" s="0"/>
       <c r="H48" s="0"/>
       <c r="I48" s="0"/>
@@ -1820,6 +1837,9 @@
       <c r="K48" s="0"/>
       <c r="L48" s="0"/>
       <c r="M48" s="0"/>
+      <c r="N48" s="0"/>
+      <c r="AMI48" s="0"/>
+      <c r="AMJ48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="46"/>
@@ -2030,13 +2050,9 @@
       <c r="L67" s="0"/>
       <c r="M67" s="0"/>
     </row>
-    <row r="68" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="46"/>
-      <c r="B68" s="0"/>
       <c r="C68" s="0"/>
-      <c r="D68" s="0"/>
-      <c r="E68" s="0"/>
-      <c r="F68" s="0"/>
       <c r="G68" s="0"/>
       <c r="H68" s="0"/>
       <c r="I68" s="0"/>
@@ -2044,9 +2060,6 @@
       <c r="K68" s="0"/>
       <c r="L68" s="0"/>
       <c r="M68" s="0"/>
-      <c r="N68" s="0"/>
-      <c r="AMI68" s="0"/>
-      <c r="AMJ68" s="0"/>
     </row>
     <row r="69" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="46"/>
@@ -2138,7 +2151,7 @@
       <c r="AMI73" s="0"/>
       <c r="AMJ73" s="0"/>
     </row>
-    <row r="74" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="46"/>
       <c r="B74" s="0"/>
       <c r="C74" s="0"/>
@@ -2156,9 +2169,13 @@
       <c r="AMI74" s="0"/>
       <c r="AMJ74" s="0"/>
     </row>
-    <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="46"/>
+      <c r="B75" s="0"/>
       <c r="C75" s="0"/>
+      <c r="D75" s="0"/>
+      <c r="E75" s="0"/>
+      <c r="F75" s="0"/>
       <c r="G75" s="0"/>
       <c r="H75" s="0"/>
       <c r="I75" s="0"/>
@@ -2166,14 +2183,13 @@
       <c r="K75" s="0"/>
       <c r="L75" s="0"/>
       <c r="M75" s="0"/>
-    </row>
-    <row r="76" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N75" s="0"/>
+      <c r="AMI75" s="0"/>
+      <c r="AMJ75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="46"/>
-      <c r="B76" s="0"/>
       <c r="C76" s="0"/>
-      <c r="D76" s="0"/>
-      <c r="E76" s="0"/>
-      <c r="F76" s="0"/>
       <c r="G76" s="0"/>
       <c r="H76" s="0"/>
       <c r="I76" s="0"/>
@@ -2181,12 +2197,9 @@
       <c r="K76" s="0"/>
       <c r="L76" s="0"/>
       <c r="M76" s="0"/>
-      <c r="N76" s="0"/>
-      <c r="AMI76" s="0"/>
-      <c r="AMJ76" s="0"/>
     </row>
     <row r="77" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="48"/>
+      <c r="A77" s="46"/>
       <c r="B77" s="0"/>
       <c r="C77" s="0"/>
       <c r="D77" s="0"/>
@@ -2365,9 +2378,13 @@
       <c r="AMI86" s="0"/>
       <c r="AMJ86" s="0"/>
     </row>
-    <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="48"/>
+      <c r="B87" s="0"/>
       <c r="C87" s="0"/>
+      <c r="D87" s="0"/>
+      <c r="E87" s="0"/>
+      <c r="F87" s="0"/>
       <c r="G87" s="0"/>
       <c r="H87" s="0"/>
       <c r="I87" s="0"/>
@@ -2375,14 +2392,13 @@
       <c r="K87" s="0"/>
       <c r="L87" s="0"/>
       <c r="M87" s="0"/>
-    </row>
-    <row r="88" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N87" s="0"/>
+      <c r="AMI87" s="0"/>
+      <c r="AMJ87" s="0"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="48"/>
-      <c r="B88" s="0"/>
       <c r="C88" s="0"/>
-      <c r="D88" s="0"/>
-      <c r="E88" s="0"/>
-      <c r="F88" s="0"/>
       <c r="G88" s="0"/>
       <c r="H88" s="0"/>
       <c r="I88" s="0"/>
@@ -2390,9 +2406,6 @@
       <c r="K88" s="0"/>
       <c r="L88" s="0"/>
       <c r="M88" s="0"/>
-      <c r="N88" s="0"/>
-      <c r="AMI88" s="0"/>
-      <c r="AMJ88" s="0"/>
     </row>
     <row r="89" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="48"/>
@@ -2448,9 +2461,13 @@
       <c r="AMI91" s="0"/>
       <c r="AMJ91" s="0"/>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="48"/>
+      <c r="B92" s="0"/>
       <c r="C92" s="0"/>
+      <c r="D92" s="0"/>
+      <c r="E92" s="0"/>
+      <c r="F92" s="0"/>
       <c r="G92" s="0"/>
       <c r="H92" s="0"/>
       <c r="I92" s="0"/>
@@ -2458,14 +2475,13 @@
       <c r="K92" s="0"/>
       <c r="L92" s="0"/>
       <c r="M92" s="0"/>
-    </row>
-    <row r="93" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N92" s="0"/>
+      <c r="AMI92" s="0"/>
+      <c r="AMJ92" s="0"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="48"/>
-      <c r="B93" s="0"/>
       <c r="C93" s="0"/>
-      <c r="D93" s="0"/>
-      <c r="E93" s="0"/>
-      <c r="F93" s="0"/>
       <c r="G93" s="0"/>
       <c r="H93" s="0"/>
       <c r="I93" s="0"/>
@@ -2473,12 +2489,9 @@
       <c r="K93" s="0"/>
       <c r="L93" s="0"/>
       <c r="M93" s="0"/>
-      <c r="N93" s="0"/>
-      <c r="AMI93" s="0"/>
-      <c r="AMJ93" s="0"/>
     </row>
     <row r="94" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="4"/>
+      <c r="A94" s="48"/>
       <c r="B94" s="0"/>
       <c r="C94" s="0"/>
       <c r="D94" s="0"/>
@@ -2549,8 +2562,13 @@
       <c r="AMI97" s="0"/>
       <c r="AMJ97" s="0"/>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="4"/>
+      <c r="B98" s="0"/>
       <c r="C98" s="0"/>
+      <c r="D98" s="0"/>
+      <c r="E98" s="0"/>
+      <c r="F98" s="0"/>
       <c r="G98" s="0"/>
       <c r="H98" s="0"/>
       <c r="I98" s="0"/>
@@ -2558,8 +2576,11 @@
       <c r="K98" s="0"/>
       <c r="L98" s="0"/>
       <c r="M98" s="0"/>
-    </row>
-    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N98" s="0"/>
+      <c r="AMI98" s="0"/>
+      <c r="AMJ98" s="0"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="0"/>
       <c r="G99" s="0"/>
       <c r="H99" s="0"/>
@@ -3169,7 +3190,16 @@
       <c r="L159" s="0"/>
       <c r="M159" s="0"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C160" s="0"/>
+      <c r="G160" s="0"/>
+      <c r="H160" s="0"/>
+      <c r="I160" s="0"/>
+      <c r="J160" s="0"/>
+      <c r="K160" s="0"/>
+      <c r="L160" s="0"/>
+      <c r="M160" s="0"/>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="18">
@@ -3178,36 +3208,36 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B8:B12"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="L11:M11"/>
-    <mergeCell ref="B12:B14"/>
     <mergeCell ref="L12:M12"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="L14:M14"/>
-    <mergeCell ref="B15:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="B16:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B37:B38"/>
   </mergeCells>
-  <conditionalFormatting sqref="C36:C37 C22:C34 C6:C20">
+  <conditionalFormatting sqref="C37:C38 C23:C35 C6:C21">
     <cfRule type="notContainsText" priority="2" operator="notContains" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="BLI" dxfId="0">
       <formula>ISERROR(SEARCH("BLI",C6))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G37 K10:K12">
+  <conditionalFormatting sqref="K11:K13 G6:G38">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="1">
-      <formula>NOT(ISERROR(SEARCH("TRUE",G6)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",G5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10:G11 G36:G37 G16:G25 G30:G31">
+  <conditionalFormatting sqref="G11:G12 G37:G38 G17:G26 G31:G32">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Pending" dxfId="2">
-      <formula>NOT(ISERROR(SEARCH("Pending",G10)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pending",G11)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Done" dxfId="3">
-      <formula>NOT(ISERROR(SEARCH("Done",G10)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Iniciar locação  não / não aproveitando reserva
</commit_message>
<xml_diff>
--- a/doc/Planejamento.xlsx
+++ b/doc/Planejamento.xlsx
@@ -70,10 +70,10 @@
     <t xml:space="preserve">Iniciar locação  não / não aproveitando reserva</t>
   </si>
   <si>
+    <t xml:space="preserve">Finalizar locação</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pendente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalizar locação</t>
   </si>
   <si>
     <t xml:space="preserve">15 min = 0,25</t>
@@ -228,12 +228,13 @@
     <numFmt numFmtId="168" formatCode="HH:MM:SS"/>
     <numFmt numFmtId="169" formatCode="0.00"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -251,29 +252,34 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -281,6 +287,28 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -288,68 +316,49 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF010000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF010000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF010000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF010000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="15">
@@ -358,30 +367,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -399,6 +384,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -476,7 +485,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -500,55 +509,52 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -557,11 +563,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -581,47 +587,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -629,7 +635,51 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -637,51 +687,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -689,7 +695,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -701,7 +707,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -741,7 +747,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,35 +756,35 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 14" xfId="20"/>
+    <cellStyle name="Accent 13" xfId="21"/>
+    <cellStyle name="Accent 2 15" xfId="22"/>
+    <cellStyle name="Accent 3 16" xfId="23"/>
+    <cellStyle name="Bad 10" xfId="24"/>
+    <cellStyle name="Error 12" xfId="25"/>
+    <cellStyle name="Footnote 5" xfId="26"/>
+    <cellStyle name="Good 8" xfId="27"/>
+    <cellStyle name="Heading 1 1" xfId="28"/>
+    <cellStyle name="Heading 2 2" xfId="29"/>
+    <cellStyle name="Hyperlink 6" xfId="30"/>
+    <cellStyle name="Neutral 9" xfId="31"/>
+    <cellStyle name="Note 4" xfId="32"/>
+    <cellStyle name="Status 7" xfId="33"/>
+    <cellStyle name="Text 3" xfId="34"/>
+    <cellStyle name="Warning 11" xfId="35"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
       <font>
         <name val="Arial"/>
+        <charset val="1"/>
         <family val="0"/>
         <color rgb="FF000000"/>
       </font>
@@ -791,6 +797,7 @@
     <dxf>
       <font>
         <name val="Arial"/>
+        <charset val="1"/>
         <family val="0"/>
         <color rgb="FF808080"/>
       </font>
@@ -803,6 +810,7 @@
     <dxf>
       <font>
         <name val="Arial"/>
+        <charset val="1"/>
         <family val="0"/>
         <color rgb="FF000000"/>
       </font>
@@ -815,6 +823,7 @@
     <dxf>
       <font>
         <name val="Arial"/>
+        <charset val="1"/>
         <family val="0"/>
         <color rgb="FF000000"/>
       </font>
@@ -895,8 +904,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -963,7 +972,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="n">
         <f aca="false">SUM(F6:F26)</f>
-        <v>14.99</v>
+        <v>44.99</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="0"/>
@@ -1120,16 +1129,18 @@
         <v>5</v>
       </c>
       <c r="E9" s="22"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="26" t="s">
-        <v>16</v>
+      <c r="F9" s="21" t="n">
+        <v>30</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
       <c r="N9" s="0"/>
       <c r="O9" s="0"/>
       <c r="P9" s="0"/>
@@ -1142,14 +1153,14 @@
         <v>4</v>
       </c>
       <c r="B10" s="19"/>
-      <c r="C10" s="28" t="s">
-        <v>17</v>
+      <c r="C10" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
       <c r="F10" s="21"/>
-      <c r="G10" s="26" t="s">
-        <v>16</v>
+      <c r="G10" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H10" s="29"/>
       <c r="I10" s="0"/>
@@ -1177,8 +1188,8 @@
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="26" t="s">
-        <v>16</v>
+      <c r="G11" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H11" s="0"/>
       <c r="I11" s="32"/>
@@ -1208,14 +1219,14 @@
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="26" t="s">
-        <v>16</v>
+      <c r="G12" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H12" s="0"/>
       <c r="I12" s="33"/>
       <c r="J12" s="33"/>
       <c r="K12" s="34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L12" s="30" t="s">
         <v>22</v>
@@ -1241,8 +1252,8 @@
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="26" t="s">
-        <v>16</v>
+      <c r="G13" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="33"/>
@@ -1272,8 +1283,8 @@
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="26" t="s">
-        <v>16</v>
+      <c r="G14" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
@@ -1298,8 +1309,8 @@
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="26" t="s">
-        <v>16</v>
+      <c r="G15" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
@@ -1323,8 +1334,8 @@
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="26" t="s">
-        <v>16</v>
+      <c r="G16" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
@@ -1344,8 +1355,8 @@
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="21"/>
-      <c r="G17" s="26" t="s">
-        <v>16</v>
+      <c r="G17" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -1368,8 +1379,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F18" s="21"/>
-      <c r="G18" s="26" t="s">
-        <v>16</v>
+      <c r="G18" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -1392,8 +1403,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F19" s="21"/>
-      <c r="G19" s="26" t="s">
-        <v>16</v>
+      <c r="G19" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -1416,8 +1427,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F20" s="21"/>
-      <c r="G20" s="26" t="s">
-        <v>16</v>
+      <c r="G20" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
@@ -1443,8 +1454,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F21" s="21"/>
-      <c r="G21" s="26" t="s">
-        <v>16</v>
+      <c r="G21" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
@@ -1467,8 +1478,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F22" s="21"/>
-      <c r="G22" s="26" t="s">
-        <v>16</v>
+      <c r="G22" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
@@ -1494,8 +1505,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F23" s="21"/>
-      <c r="G23" s="26" t="s">
-        <v>16</v>
+      <c r="G23" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
@@ -1518,8 +1529,8 @@
       <c r="D24" s="21"/>
       <c r="E24" s="22"/>
       <c r="F24" s="21"/>
-      <c r="G24" s="26" t="s">
-        <v>16</v>
+      <c r="G24" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
@@ -1542,8 +1553,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F25" s="21"/>
-      <c r="G25" s="26" t="s">
-        <v>16</v>
+      <c r="G25" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
@@ -1566,8 +1577,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F26" s="21"/>
-      <c r="G26" s="26" t="s">
-        <v>16</v>
+      <c r="G26" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H26" s="0"/>
       <c r="I26" s="0"/>
@@ -1590,8 +1601,8 @@
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="21"/>
-      <c r="G27" s="26" t="s">
-        <v>16</v>
+      <c r="G27" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
@@ -1612,8 +1623,8 @@
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="21"/>
-      <c r="G28" s="26" t="s">
-        <v>16</v>
+      <c r="G28" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H28" s="0"/>
       <c r="I28" s="0"/>
@@ -1636,8 +1647,8 @@
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
       <c r="F29" s="21"/>
-      <c r="G29" s="26" t="s">
-        <v>16</v>
+      <c r="G29" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H29" s="0"/>
       <c r="I29" s="0"/>
@@ -1658,8 +1669,8 @@
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
       <c r="F30" s="21"/>
-      <c r="G30" s="26" t="s">
-        <v>16</v>
+      <c r="G30" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H30" s="0"/>
       <c r="I30" s="0"/>
@@ -1680,8 +1691,8 @@
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
       <c r="F31" s="21"/>
-      <c r="G31" s="26" t="s">
-        <v>16</v>
+      <c r="G31" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
@@ -1702,8 +1713,8 @@
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
       <c r="F32" s="21"/>
-      <c r="G32" s="26" t="s">
-        <v>16</v>
+      <c r="G32" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H32" s="0"/>
       <c r="I32" s="0"/>
@@ -1726,8 +1737,8 @@
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
       <c r="F33" s="21"/>
-      <c r="G33" s="26" t="s">
-        <v>16</v>
+      <c r="G33" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
@@ -1748,8 +1759,8 @@
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
       <c r="F34" s="21"/>
-      <c r="G34" s="26" t="s">
-        <v>16</v>
+      <c r="G34" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H34" s="0"/>
       <c r="I34" s="0"/>
@@ -1772,8 +1783,8 @@
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="21"/>
-      <c r="G35" s="26" t="s">
-        <v>16</v>
+      <c r="G35" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
@@ -1796,8 +1807,8 @@
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="21"/>
-      <c r="G36" s="26" t="s">
-        <v>16</v>
+      <c r="G36" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H36" s="0"/>
       <c r="I36" s="0"/>
@@ -1820,8 +1831,8 @@
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
       <c r="F37" s="21"/>
-      <c r="G37" s="26" t="s">
-        <v>16</v>
+      <c r="G37" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H37" s="0"/>
       <c r="I37" s="0"/>
@@ -1842,8 +1853,8 @@
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
       <c r="F38" s="21"/>
-      <c r="G38" s="26" t="s">
-        <v>16</v>
+      <c r="G38" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="H38" s="0"/>
       <c r="I38" s="0"/>

</xml_diff>

<commit_message>
Busca por busca aprimorada a genericidade; estender visualização de disponibilidade reserva para também locação
</commit_message>
<xml_diff>
--- a/doc/Planejamento.xlsx
+++ b/doc/Planejamento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t xml:space="preserve">Planejado</t>
   </si>
@@ -67,95 +67,98 @@
     <t xml:space="preserve">Buscar categorias de veiculo superiores</t>
   </si>
   <si>
+    <t xml:space="preserve">Listar motoristas validos para locação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar veículos disponíveis para locação  por filial/ filial e categoria</t>
+  </si>
+  <si>
     <t xml:space="preserve">Iniciar locação  não / não aproveitando reserva</t>
   </si>
   <si>
+    <t xml:space="preserve">estender visualização de disponibilidade reserva para também locação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em Curso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estender visualização acompanhamento reserva para também locação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar veículos com locação em progresso por filial/cliente pela filial</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finalizar locação</t>
   </si>
   <si>
+    <t xml:space="preserve">Manutenção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar veículos pendentes  </t>
+  </si>
+  <si>
     <t xml:space="preserve">Pendente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 min = 0,25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listar veículos disponíveis para locação  por filial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 min = 0,16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listar veículos com locação em progresso por pela filial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 min = 0,33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manutenção</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listar veículos pendentes  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Em Curso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 min = 0,50</t>
   </si>
   <si>
     <t xml:space="preserve">Listar veículos em manutenção
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Mandar manualmente para revisão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relatórios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estudar iReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Histórico de manutenção por veículo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clientes por tipo físico / jurídico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 min = 0,25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reserva por período</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 min = 0,16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locação por período</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 min = 0,33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locação por cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 min = 0,50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locação por motorista</t>
+  </si>
+  <si>
     <t xml:space="preserve">40 min = 0,66</t>
   </si>
   <si>
-    <t xml:space="preserve">Mandar manualmente para revisão
-</t>
+    <t xml:space="preserve">financeiro- reservas canceladas(dinheiro em potencial perdido) reservas efetuadas, por período</t>
   </si>
   <si>
     <t xml:space="preserve">50 min = 0,83</t>
   </si>
   <si>
-    <t xml:space="preserve">Relatórios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estudar iReport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Histórico de manutenção por veículo
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clientes por tipo físico / jurídico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reserva por período
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locação por período</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locação por cliente
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locação por motorista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">financeiro- reservas canceladas(dinheiro em potencial perdido) reservas efetuadas, por período</t>
-  </si>
-  <si>
     <t xml:space="preserve">implementar no DaoRes salvamento de relatório para caminho especificado</t>
   </si>
   <si>
-    <t xml:space="preserve">locações/reservas por funcionário e período
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locações/reservas por filial e período
-</t>
+    <t xml:space="preserve">locações/reservas por funcionário e período</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locações/reservas por filial e período</t>
   </si>
   <si>
     <t xml:space="preserve">Auditoria</t>
@@ -164,22 +167,19 @@
     <t xml:space="preserve">criação de tigger, procedure e tebela de log </t>
   </si>
   <si>
-    <t xml:space="preserve">criação de tela para visualização de log por período para adms
-</t>
+    <t xml:space="preserve">criação de tela para visualização de log por período para adms</t>
   </si>
   <si>
     <t xml:space="preserve">Cadastro simplificado</t>
   </si>
   <si>
-    <t xml:space="preserve">cliente físico
-</t>
+    <t xml:space="preserve">cliente físico</t>
   </si>
   <si>
     <t xml:space="preserve">cliente jurídico</t>
   </si>
   <si>
-    <t xml:space="preserve">Automóvel
-</t>
+    <t xml:space="preserve">Automóvel</t>
   </si>
   <si>
     <t xml:space="preserve">caminhonete carga</t>
@@ -188,8 +188,7 @@
     <t xml:space="preserve">Backup</t>
   </si>
   <si>
-    <t xml:space="preserve">pesquisar como definir hora para backup em banco
-</t>
+    <t xml:space="preserve">pesquisar como definir hora para backup em banco</t>
   </si>
   <si>
     <t xml:space="preserve">utilizar procedure ?</t>
@@ -436,14 +435,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -640,7 +639,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -667,80 +666,80 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -780,7 +779,7 @@
     <cellStyle name="Text 3" xfId="34"/>
     <cellStyle name="Warning 11" xfId="35"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="1">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -788,50 +787,7 @@
         <family val="0"/>
         <color rgb="FF000000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF808080"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF808080"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -902,10 +858,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:AMJ163"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -966,12 +922,12 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="10" t="n">
-        <f aca="false">SUM(D6:D26)</f>
-        <v>12</v>
+        <f aca="false">SUM(D6:D29)</f>
+        <v>26</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="n">
-        <f aca="false">SUM(F6:F26)</f>
+        <f aca="false">SUM(F6:F29)</f>
         <v>44.99</v>
       </c>
       <c r="G3" s="12"/>
@@ -1118,19 +1074,17 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="n">
-        <v>3</v>
-      </c>
+      <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="21" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="21" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>11</v>
@@ -1148,29 +1102,31 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="21" t="n">
+        <v>2</v>
+      </c>
       <c r="E10" s="22"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="29"/>
-      <c r="I10" s="0"/>
-      <c r="J10" s="0"/>
+      <c r="F10" s="21" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="0"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
       <c r="K10" s="0"/>
-      <c r="L10" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="8"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="0"/>
       <c r="O10" s="0"/>
       <c r="P10" s="0"/>
       <c r="Q10" s="0"/>
@@ -1178,29 +1134,27 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="n">
-        <v>5</v>
-      </c>
+      <c r="A11" s="18"/>
       <c r="B11" s="19"/>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="21" t="n">
         <v>19</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="28" t="s">
-        <v>17</v>
+      <c r="G11" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H11" s="0"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="30"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
       <c r="N11" s="0"/>
       <c r="O11" s="0"/>
       <c r="P11" s="0"/>
@@ -1208,63 +1162,53 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="n">
-        <v>6</v>
-      </c>
+    <row r="12" s="2" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="21"/>
+        <v>18</v>
+      </c>
+      <c r="D12" s="21" t="n">
+        <v>2</v>
+      </c>
       <c r="E12" s="22"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="0"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" s="30"/>
+      <c r="G12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="30" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
       <c r="N12" s="0"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
       <c r="AMI12" s="0"/>
       <c r="AMJ12" s="0"/>
     </row>
-    <row r="13" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="n">
-        <v>7</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>23</v>
-      </c>
+    <row r="13" s="2" customFormat="true" ht="24.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="28" t="s">
-        <v>17</v>
+      <c r="G13" s="29" t="s">
+        <v>19</v>
       </c>
       <c r="H13" s="0"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="30"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
       <c r="N13" s="0"/>
       <c r="O13" s="0"/>
       <c r="P13" s="0"/>
@@ -1272,91 +1216,102 @@
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="2" customFormat="true" ht="19.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="n">
-        <v>8</v>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="31" t="s">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="28" t="s">
-        <v>17</v>
+      <c r="G14" s="29" t="s">
+        <v>19</v>
       </c>
       <c r="H14" s="0"/>
-      <c r="I14" s="0"/>
-      <c r="J14" s="0"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
       <c r="K14" s="0"/>
-      <c r="L14" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="M14" s="30"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
       <c r="N14" s="0"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="n">
-        <v>9</v>
-      </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="21"/>
+    <row r="15" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="21" t="n">
+        <v>10</v>
+      </c>
       <c r="E15" s="22"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="28" t="s">
-        <v>17</v>
+      <c r="G15" s="29" t="s">
+        <v>19</v>
       </c>
       <c r="H15" s="0"/>
-      <c r="I15" s="0"/>
-      <c r="J15" s="0"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
       <c r="K15" s="0"/>
-      <c r="L15" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="M15" s="30"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L15" s="0"/>
+      <c r="M15" s="0"/>
+      <c r="N15" s="0"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="AMI15" s="0"/>
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row r="16" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="n">
-        <v>10</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="28" t="s">
-        <v>17</v>
+      <c r="G16" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H16" s="0"/>
-      <c r="I16" s="0"/>
-      <c r="J16" s="0"/>
-      <c r="K16" s="29"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="0"/>
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N16" s="0"/>
+      <c r="O16" s="0"/>
+      <c r="P16" s="0"/>
+      <c r="Q16" s="0"/>
+      <c r="AMI16" s="0"/>
+      <c r="AMJ16" s="0"/>
+    </row>
+    <row r="17" s="2" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="n">
-        <v>11</v>
-      </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="31" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="27" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="21"/>
-      <c r="G17" s="28" t="s">
-        <v>17</v>
+      <c r="G17" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -1364,23 +1319,23 @@
       <c r="K17" s="0"/>
       <c r="L17" s="0"/>
       <c r="M17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N17" s="0"/>
+      <c r="AMI17" s="0"/>
+      <c r="AMJ17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="16.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="n">
-        <v>12</v>
-      </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="39" t="s">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="27" t="s">
+        <v>27</v>
       </c>
       <c r="D18" s="21"/>
-      <c r="E18" s="22" t="e">
-        <f aca="false">C19*D18</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="E18" s="22"/>
       <c r="F18" s="21"/>
-      <c r="G18" s="28" t="s">
-        <v>17</v>
+      <c r="G18" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -1389,22 +1344,21 @@
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
     </row>
-    <row r="19" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="n">
-        <v>13</v>
-      </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="31" t="s">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>29</v>
       </c>
       <c r="D19" s="21"/>
-      <c r="E19" s="22" t="e">
-        <f aca="false">C20*D19</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="E19" s="22"/>
       <c r="F19" s="21"/>
-      <c r="G19" s="28" t="s">
-        <v>17</v>
+      <c r="G19" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -1413,22 +1367,19 @@
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
     </row>
-    <row r="20" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="18.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="n">
-        <v>14</v>
-      </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="31" t="s">
-        <v>36</v>
+        <v>11</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="D20" s="21"/>
-      <c r="E20" s="22" t="e">
-        <f aca="false">C21*D20</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="E20" s="22"/>
       <c r="F20" s="21"/>
-      <c r="G20" s="28" t="s">
-        <v>17</v>
+      <c r="G20" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
@@ -1436,41 +1387,41 @@
       <c r="K20" s="0"/>
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
-      <c r="N20" s="0"/>
-      <c r="AMI20" s="0"/>
-      <c r="AMJ20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="n">
-        <v>15</v>
-      </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="31" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="37" t="s">
+        <v>31</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="22" t="e">
-        <f aca="false">C23*D21</f>
+        <f aca="false">C22*D21</f>
         <v>#VALUE!</v>
       </c>
       <c r="F21" s="21"/>
-      <c r="G21" s="28" t="s">
-        <v>17</v>
+      <c r="G21" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
       <c r="K21" s="0"/>
       <c r="L21" s="0"/>
-      <c r="M21" s="0"/>
-    </row>
-    <row r="22" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M21" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="N21" s="38"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="n">
-        <v>16</v>
-      </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="40" t="s">
-        <v>38</v>
+        <v>13</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="27" t="s">
+        <v>33</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="22" t="e">
@@ -1478,26 +1429,28 @@
         <v>#VALUE!</v>
       </c>
       <c r="F22" s="21"/>
-      <c r="G22" s="28" t="s">
-        <v>17</v>
+      <c r="G22" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
-      <c r="L22" s="0"/>
-      <c r="M22" s="0"/>
-      <c r="N22" s="0"/>
-      <c r="AMI22" s="0"/>
-      <c r="AMJ22" s="0"/>
-    </row>
-    <row r="23" s="2" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L22" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" s="38"/>
+    </row>
+    <row r="23" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="31" t="s">
-        <v>39</v>
+        <v>14</v>
+      </c>
+      <c r="B23" s="34"/>
+      <c r="C23" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="22" t="e">
@@ -1505,126 +1458,147 @@
         <v>#VALUE!</v>
       </c>
       <c r="F23" s="21"/>
-      <c r="G23" s="28" t="s">
-        <v>17</v>
+      <c r="G23" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
-      <c r="L23" s="0"/>
-      <c r="M23" s="0"/>
-      <c r="N23" s="0"/>
+      <c r="L23" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="N23" s="38"/>
       <c r="AMI23" s="0"/>
       <c r="AMJ23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="n">
-        <v>18</v>
-      </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="41" t="s">
-        <v>40</v>
+        <v>15</v>
+      </c>
+      <c r="B24" s="34"/>
+      <c r="C24" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
+      <c r="E24" s="22" t="e">
+        <f aca="false">C26*D24</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="F24" s="21"/>
-      <c r="G24" s="28" t="s">
-        <v>17</v>
+      <c r="G24" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
-      <c r="L24" s="0"/>
-      <c r="M24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L24" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="N24" s="38"/>
+    </row>
+    <row r="25" s="2" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="n">
-        <v>19</v>
-      </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="41" t="s">
-        <v>41</v>
+        <v>16</v>
+      </c>
+      <c r="B25" s="34"/>
+      <c r="C25" s="40" t="s">
+        <v>39</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="22" t="e">
-        <f aca="false">C25*D25</f>
+        <f aca="false">C26*D25</f>
         <v>#VALUE!</v>
       </c>
       <c r="F25" s="21"/>
-      <c r="G25" s="28" t="s">
-        <v>17</v>
+      <c r="G25" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
       <c r="L25" s="0"/>
-      <c r="M25" s="0"/>
-    </row>
-    <row r="26" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M25" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="N25" s="38"/>
+      <c r="AMI25" s="0"/>
+      <c r="AMJ25" s="0"/>
+    </row>
+    <row r="26" s="2" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="n">
-        <v>20</v>
-      </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="41" t="s">
-        <v>42</v>
+        <v>17</v>
+      </c>
+      <c r="B26" s="34"/>
+      <c r="C26" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="22" t="e">
-        <f aca="false">C26*D26</f>
+        <f aca="false">C27*D26</f>
         <v>#VALUE!</v>
       </c>
       <c r="F26" s="21"/>
-      <c r="G26" s="28" t="s">
-        <v>17</v>
+      <c r="G26" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H26" s="0"/>
       <c r="I26" s="0"/>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
       <c r="L26" s="0"/>
-      <c r="M26" s="0"/>
-      <c r="N26" s="0"/>
+      <c r="M26" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" s="38"/>
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
-    <row r="27" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18"/>
-      <c r="B27" s="36" t="s">
+    <row r="27" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B27" s="34"/>
+      <c r="C27" s="41" t="s">
         <v>43</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>44</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="21"/>
-      <c r="G27" s="28" t="s">
-        <v>17</v>
+      <c r="G27" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
       <c r="J27" s="0"/>
       <c r="K27" s="0"/>
-      <c r="L27" s="0"/>
+      <c r="L27" s="42"/>
       <c r="M27" s="0"/>
-      <c r="N27" s="0"/>
-      <c r="AMI27" s="0"/>
-      <c r="AMJ27" s="0"/>
-    </row>
-    <row r="28" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18"/>
-      <c r="B28" s="36"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="18" t="n">
+        <v>19</v>
+      </c>
+      <c r="B28" s="34"/>
       <c r="C28" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="21"/>
-      <c r="E28" s="22"/>
+      <c r="E28" s="22" t="e">
+        <f aca="false">C28*D28</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="F28" s="21"/>
-      <c r="G28" s="28" t="s">
-        <v>17</v>
+      <c r="G28" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H28" s="0"/>
       <c r="I28" s="0"/>
@@ -1632,23 +1606,23 @@
       <c r="K28" s="0"/>
       <c r="L28" s="0"/>
       <c r="M28" s="0"/>
-      <c r="N28" s="0"/>
-      <c r="AMI28" s="0"/>
-      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
-      <c r="B29" s="36" t="s">
-        <v>46</v>
-      </c>
+      <c r="A29" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="B29" s="34"/>
       <c r="C29" s="41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D29" s="21"/>
-      <c r="E29" s="22"/>
+      <c r="E29" s="22" t="e">
+        <f aca="false">C29*D29</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="F29" s="21"/>
-      <c r="G29" s="28" t="s">
-        <v>17</v>
+      <c r="G29" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H29" s="0"/>
       <c r="I29" s="0"/>
@@ -1662,15 +1636,17 @@
     </row>
     <row r="30" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
-      <c r="B30" s="36"/>
+      <c r="B30" s="34" t="s">
+        <v>46</v>
+      </c>
       <c r="C30" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
       <c r="F30" s="21"/>
-      <c r="G30" s="28" t="s">
-        <v>17</v>
+      <c r="G30" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H30" s="0"/>
       <c r="I30" s="0"/>
@@ -1684,15 +1660,15 @@
     </row>
     <row r="31" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
-      <c r="B31" s="36"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
       <c r="F31" s="21"/>
-      <c r="G31" s="28" t="s">
-        <v>17</v>
+      <c r="G31" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
@@ -1706,15 +1682,17 @@
     </row>
     <row r="32" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="42" t="s">
+      <c r="B32" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="41" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
       <c r="F32" s="21"/>
-      <c r="G32" s="28" t="s">
-        <v>17</v>
+      <c r="G32" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H32" s="0"/>
       <c r="I32" s="0"/>
@@ -1728,17 +1706,15 @@
     </row>
     <row r="33" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="34"/>
+      <c r="C33" s="41" t="s">
         <v>51</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>52</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
       <c r="F33" s="21"/>
-      <c r="G33" s="28" t="s">
-        <v>17</v>
+      <c r="G33" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
@@ -1752,15 +1728,15 @@
     </row>
     <row r="34" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
-      <c r="B34" s="36"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
       <c r="F34" s="21"/>
-      <c r="G34" s="28" t="s">
-        <v>17</v>
+      <c r="G34" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H34" s="0"/>
       <c r="I34" s="0"/>
@@ -1772,19 +1748,17 @@
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
-      <c r="B35" s="36" t="s">
-        <v>54</v>
-      </c>
+      <c r="B35" s="34"/>
       <c r="C35" s="43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="21"/>
-      <c r="G35" s="28" t="s">
-        <v>17</v>
+      <c r="G35" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
@@ -1796,19 +1770,19 @@
       <c r="AMI35" s="0"/>
       <c r="AMJ35" s="0"/>
     </row>
-    <row r="36" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
-      <c r="B36" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="45" t="s">
-        <v>57</v>
+      <c r="B36" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>55</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="21"/>
-      <c r="G36" s="28" t="s">
-        <v>17</v>
+      <c r="G36" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H36" s="0"/>
       <c r="I36" s="0"/>
@@ -1820,19 +1794,17 @@
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
-      <c r="B37" s="36" t="s">
-        <v>58</v>
-      </c>
+      <c r="B37" s="34"/>
       <c r="C37" s="41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
       <c r="F37" s="21"/>
-      <c r="G37" s="28" t="s">
-        <v>17</v>
+      <c r="G37" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H37" s="0"/>
       <c r="I37" s="0"/>
@@ -1846,15 +1818,17 @@
     </row>
     <row r="38" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="41" t="s">
-        <v>60</v>
+      <c r="B38" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>58</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
       <c r="F38" s="21"/>
-      <c r="G38" s="28" t="s">
-        <v>17</v>
+      <c r="G38" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="H38" s="0"/>
       <c r="I38" s="0"/>
@@ -1866,14 +1840,20 @@
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="46"/>
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
-      <c r="D39" s="0"/>
-      <c r="E39" s="0"/>
-      <c r="F39" s="0"/>
-      <c r="G39" s="0"/>
+    <row r="39" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="18"/>
+      <c r="B39" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="21"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="35" t="s">
+        <v>25</v>
+      </c>
       <c r="H39" s="0"/>
       <c r="I39" s="0"/>
       <c r="J39" s="0"/>
@@ -1884,14 +1864,20 @@
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="46"/>
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
-      <c r="F40" s="0"/>
-      <c r="G40" s="0"/>
+    <row r="40" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="18"/>
+      <c r="B40" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="21"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="35" t="s">
+        <v>25</v>
+      </c>
       <c r="H40" s="0"/>
       <c r="I40" s="0"/>
       <c r="J40" s="0"/>
@@ -1902,14 +1888,18 @@
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
-    <row r="41" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="46"/>
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
-      <c r="D41" s="0"/>
-      <c r="E41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
+    <row r="41" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="18"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="35" t="s">
+        <v>25</v>
+      </c>
       <c r="H41" s="0"/>
       <c r="I41" s="0"/>
       <c r="J41" s="0"/>
@@ -1956,7 +1946,7 @@
       <c r="AMI43" s="0"/>
       <c r="AMJ43" s="0"/>
     </row>
-    <row r="44" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="46"/>
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
@@ -1974,7 +1964,7 @@
       <c r="AMI44" s="0"/>
       <c r="AMJ44" s="0"/>
     </row>
-    <row r="45" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="46"/>
       <c r="B45" s="0"/>
       <c r="C45" s="0"/>
@@ -1992,7 +1982,7 @@
       <c r="AMI45" s="0"/>
       <c r="AMJ45" s="0"/>
     </row>
-    <row r="46" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="46"/>
       <c r="B46" s="0"/>
       <c r="C46" s="0"/>
@@ -2046,9 +2036,13 @@
       <c r="AMI48" s="0"/>
       <c r="AMJ48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="46"/>
+      <c r="B49" s="0"/>
       <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
+      <c r="F49" s="0"/>
       <c r="G49" s="0"/>
       <c r="H49" s="0"/>
       <c r="I49" s="0"/>
@@ -2056,10 +2050,17 @@
       <c r="K49" s="0"/>
       <c r="L49" s="0"/>
       <c r="M49" s="0"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N49" s="0"/>
+      <c r="AMI49" s="0"/>
+      <c r="AMJ49" s="0"/>
+    </row>
+    <row r="50" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="46"/>
+      <c r="B50" s="0"/>
       <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
       <c r="G50" s="0"/>
       <c r="H50" s="0"/>
       <c r="I50" s="0"/>
@@ -2067,10 +2068,17 @@
       <c r="K50" s="0"/>
       <c r="L50" s="0"/>
       <c r="M50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N50" s="0"/>
+      <c r="AMI50" s="0"/>
+      <c r="AMJ50" s="0"/>
+    </row>
+    <row r="51" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="46"/>
+      <c r="B51" s="0"/>
       <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
+      <c r="F51" s="0"/>
       <c r="G51" s="0"/>
       <c r="H51" s="0"/>
       <c r="I51" s="0"/>
@@ -2078,6 +2086,9 @@
       <c r="K51" s="0"/>
       <c r="L51" s="0"/>
       <c r="M51" s="0"/>
+      <c r="N51" s="0"/>
+      <c r="AMI51" s="0"/>
+      <c r="AMJ51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="46"/>
@@ -2266,13 +2277,9 @@
       <c r="L68" s="0"/>
       <c r="M68" s="0"/>
     </row>
-    <row r="69" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="46"/>
-      <c r="B69" s="0"/>
       <c r="C69" s="0"/>
-      <c r="D69" s="0"/>
-      <c r="E69" s="0"/>
-      <c r="F69" s="0"/>
       <c r="G69" s="0"/>
       <c r="H69" s="0"/>
       <c r="I69" s="0"/>
@@ -2280,17 +2287,10 @@
       <c r="K69" s="0"/>
       <c r="L69" s="0"/>
       <c r="M69" s="0"/>
-      <c r="N69" s="0"/>
-      <c r="AMI69" s="0"/>
-      <c r="AMJ69" s="0"/>
-    </row>
-    <row r="70" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="46"/>
-      <c r="B70" s="0"/>
       <c r="C70" s="0"/>
-      <c r="D70" s="0"/>
-      <c r="E70" s="0"/>
-      <c r="F70" s="0"/>
       <c r="G70" s="0"/>
       <c r="H70" s="0"/>
       <c r="I70" s="0"/>
@@ -2298,17 +2298,10 @@
       <c r="K70" s="0"/>
       <c r="L70" s="0"/>
       <c r="M70" s="0"/>
-      <c r="N70" s="0"/>
-      <c r="AMI70" s="0"/>
-      <c r="AMJ70" s="0"/>
-    </row>
-    <row r="71" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="46"/>
-      <c r="B71" s="0"/>
       <c r="C71" s="0"/>
-      <c r="D71" s="0"/>
-      <c r="E71" s="0"/>
-      <c r="F71" s="0"/>
       <c r="G71" s="0"/>
       <c r="H71" s="0"/>
       <c r="I71" s="0"/>
@@ -2316,9 +2309,6 @@
       <c r="K71" s="0"/>
       <c r="L71" s="0"/>
       <c r="M71" s="0"/>
-      <c r="N71" s="0"/>
-      <c r="AMI71" s="0"/>
-      <c r="AMJ71" s="0"/>
     </row>
     <row r="72" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="46"/>
@@ -2374,7 +2364,7 @@
       <c r="AMI74" s="0"/>
       <c r="AMJ74" s="0"/>
     </row>
-    <row r="75" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="46"/>
       <c r="B75" s="0"/>
       <c r="C75" s="0"/>
@@ -2392,9 +2382,13 @@
       <c r="AMI75" s="0"/>
       <c r="AMJ75" s="0"/>
     </row>
-    <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="46"/>
+      <c r="B76" s="0"/>
       <c r="C76" s="0"/>
+      <c r="D76" s="0"/>
+      <c r="E76" s="0"/>
+      <c r="F76" s="0"/>
       <c r="G76" s="0"/>
       <c r="H76" s="0"/>
       <c r="I76" s="0"/>
@@ -2402,6 +2396,9 @@
       <c r="K76" s="0"/>
       <c r="L76" s="0"/>
       <c r="M76" s="0"/>
+      <c r="N76" s="0"/>
+      <c r="AMI76" s="0"/>
+      <c r="AMJ76" s="0"/>
     </row>
     <row r="77" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="46"/>
@@ -2421,8 +2418,8 @@
       <c r="AMI77" s="0"/>
       <c r="AMJ77" s="0"/>
     </row>
-    <row r="78" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="48"/>
+    <row r="78" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="46"/>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
@@ -2439,13 +2436,9 @@
       <c r="AMI78" s="0"/>
       <c r="AMJ78" s="0"/>
     </row>
-    <row r="79" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="48"/>
-      <c r="B79" s="0"/>
+    <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="46"/>
       <c r="C79" s="0"/>
-      <c r="D79" s="0"/>
-      <c r="E79" s="0"/>
-      <c r="F79" s="0"/>
       <c r="G79" s="0"/>
       <c r="H79" s="0"/>
       <c r="I79" s="0"/>
@@ -2453,12 +2446,9 @@
       <c r="K79" s="0"/>
       <c r="L79" s="0"/>
       <c r="M79" s="0"/>
-      <c r="N79" s="0"/>
-      <c r="AMI79" s="0"/>
-      <c r="AMJ79" s="0"/>
     </row>
     <row r="80" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="48"/>
+      <c r="A80" s="46"/>
       <c r="B80" s="0"/>
       <c r="C80" s="0"/>
       <c r="D80" s="0"/>
@@ -2601,9 +2591,13 @@
       <c r="AMI87" s="0"/>
       <c r="AMJ87" s="0"/>
     </row>
-    <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="48"/>
+      <c r="B88" s="0"/>
       <c r="C88" s="0"/>
+      <c r="D88" s="0"/>
+      <c r="E88" s="0"/>
+      <c r="F88" s="0"/>
       <c r="G88" s="0"/>
       <c r="H88" s="0"/>
       <c r="I88" s="0"/>
@@ -2611,6 +2605,9 @@
       <c r="K88" s="0"/>
       <c r="L88" s="0"/>
       <c r="M88" s="0"/>
+      <c r="N88" s="0"/>
+      <c r="AMI88" s="0"/>
+      <c r="AMJ88" s="0"/>
     </row>
     <row r="89" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="48"/>
@@ -2648,13 +2645,9 @@
       <c r="AMI90" s="0"/>
       <c r="AMJ90" s="0"/>
     </row>
-    <row r="91" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="48"/>
-      <c r="B91" s="0"/>
       <c r="C91" s="0"/>
-      <c r="D91" s="0"/>
-      <c r="E91" s="0"/>
-      <c r="F91" s="0"/>
       <c r="G91" s="0"/>
       <c r="H91" s="0"/>
       <c r="I91" s="0"/>
@@ -2662,9 +2655,6 @@
       <c r="K91" s="0"/>
       <c r="L91" s="0"/>
       <c r="M91" s="0"/>
-      <c r="N91" s="0"/>
-      <c r="AMI91" s="0"/>
-      <c r="AMJ91" s="0"/>
     </row>
     <row r="92" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="48"/>
@@ -2684,9 +2674,13 @@
       <c r="AMI92" s="0"/>
       <c r="AMJ92" s="0"/>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="48"/>
+      <c r="B93" s="0"/>
       <c r="C93" s="0"/>
+      <c r="D93" s="0"/>
+      <c r="E93" s="0"/>
+      <c r="F93" s="0"/>
       <c r="G93" s="0"/>
       <c r="H93" s="0"/>
       <c r="I93" s="0"/>
@@ -2694,6 +2688,9 @@
       <c r="K93" s="0"/>
       <c r="L93" s="0"/>
       <c r="M93" s="0"/>
+      <c r="N93" s="0"/>
+      <c r="AMI93" s="0"/>
+      <c r="AMJ93" s="0"/>
     </row>
     <row r="94" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="48"/>
@@ -2714,7 +2711,7 @@
       <c r="AMJ94" s="0"/>
     </row>
     <row r="95" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="4"/>
+      <c r="A95" s="48"/>
       <c r="B95" s="0"/>
       <c r="C95" s="0"/>
       <c r="D95" s="0"/>
@@ -2731,13 +2728,9 @@
       <c r="AMI95" s="0"/>
       <c r="AMJ95" s="0"/>
     </row>
-    <row r="96" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="4"/>
-      <c r="B96" s="0"/>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="48"/>
       <c r="C96" s="0"/>
-      <c r="D96" s="0"/>
-      <c r="E96" s="0"/>
-      <c r="F96" s="0"/>
       <c r="G96" s="0"/>
       <c r="H96" s="0"/>
       <c r="I96" s="0"/>
@@ -2745,12 +2738,9 @@
       <c r="K96" s="0"/>
       <c r="L96" s="0"/>
       <c r="M96" s="0"/>
-      <c r="N96" s="0"/>
-      <c r="AMI96" s="0"/>
-      <c r="AMJ96" s="0"/>
     </row>
     <row r="97" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="4"/>
+      <c r="A97" s="48"/>
       <c r="B97" s="0"/>
       <c r="C97" s="0"/>
       <c r="D97" s="0"/>
@@ -2785,8 +2775,13 @@
       <c r="AMI98" s="0"/>
       <c r="AMJ98" s="0"/>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="4"/>
+      <c r="B99" s="0"/>
       <c r="C99" s="0"/>
+      <c r="D99" s="0"/>
+      <c r="E99" s="0"/>
+      <c r="F99" s="0"/>
       <c r="G99" s="0"/>
       <c r="H99" s="0"/>
       <c r="I99" s="0"/>
@@ -2794,9 +2789,17 @@
       <c r="K99" s="0"/>
       <c r="L99" s="0"/>
       <c r="M99" s="0"/>
-    </row>
-    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N99" s="0"/>
+      <c r="AMI99" s="0"/>
+      <c r="AMJ99" s="0"/>
+    </row>
+    <row r="100" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="4"/>
+      <c r="B100" s="0"/>
       <c r="C100" s="0"/>
+      <c r="D100" s="0"/>
+      <c r="E100" s="0"/>
+      <c r="F100" s="0"/>
       <c r="G100" s="0"/>
       <c r="H100" s="0"/>
       <c r="I100" s="0"/>
@@ -2804,9 +2807,17 @@
       <c r="K100" s="0"/>
       <c r="L100" s="0"/>
       <c r="M100" s="0"/>
-    </row>
-    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N100" s="0"/>
+      <c r="AMI100" s="0"/>
+      <c r="AMJ100" s="0"/>
+    </row>
+    <row r="101" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="4"/>
+      <c r="B101" s="0"/>
       <c r="C101" s="0"/>
+      <c r="D101" s="0"/>
+      <c r="E101" s="0"/>
+      <c r="F101" s="0"/>
       <c r="G101" s="0"/>
       <c r="H101" s="0"/>
       <c r="I101" s="0"/>
@@ -2814,8 +2825,11 @@
       <c r="K101" s="0"/>
       <c r="L101" s="0"/>
       <c r="M101" s="0"/>
-    </row>
-    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N101" s="0"/>
+      <c r="AMI101" s="0"/>
+      <c r="AMJ101" s="0"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="0"/>
       <c r="G102" s="0"/>
       <c r="H102" s="0"/>
@@ -3405,7 +3419,36 @@
       <c r="L160" s="0"/>
       <c r="M160" s="0"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C161" s="0"/>
+      <c r="G161" s="0"/>
+      <c r="H161" s="0"/>
+      <c r="I161" s="0"/>
+      <c r="J161" s="0"/>
+      <c r="K161" s="0"/>
+      <c r="L161" s="0"/>
+      <c r="M161" s="0"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C162" s="0"/>
+      <c r="G162" s="0"/>
+      <c r="H162" s="0"/>
+      <c r="I162" s="0"/>
+      <c r="J162" s="0"/>
+      <c r="K162" s="0"/>
+      <c r="L162" s="0"/>
+      <c r="M162" s="0"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C163" s="0"/>
+      <c r="G163" s="0"/>
+      <c r="H163" s="0"/>
+      <c r="I163" s="0"/>
+      <c r="J163" s="0"/>
+      <c r="K163" s="0"/>
+      <c r="L163" s="0"/>
+      <c r="M163" s="0"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="B1:N1"/>
@@ -3413,36 +3456,36 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="B16:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B29"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B40:B41"/>
   </mergeCells>
-  <conditionalFormatting sqref="C37:C38 C23:C35 C6:C21">
+  <conditionalFormatting sqref="C40:C41 C26:C38 C6:C24">
     <cfRule type="notContainsText" priority="2" operator="notContains" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="BLI" dxfId="0">
       <formula>ISERROR(SEARCH("BLI",C6))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11:K13 G6:G38">
-    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="1">
+  <conditionalFormatting sqref="L22:L24 G6:G41">
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("TRUE",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G12 G37:G38 G17:G26 G31:G32">
-    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Pending" dxfId="2">
-      <formula>NOT(ISERROR(SEARCH("Pending",G11)))</formula>
+  <conditionalFormatting sqref="G40:G41 G20:G29 G34:G35">
+    <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Pending" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("Pending",G20)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Done" dxfId="3">
-      <formula>NOT(ISERROR(SEARCH("Done",G11)))</formula>
+    <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Done" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("Done",G20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
busca otimizada locação/ reserva, acompanhaento locação extendido
</commit_message>
<xml_diff>
--- a/doc/Planejamento.xlsx
+++ b/doc/Planejamento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t xml:space="preserve">Planejado</t>
   </si>
@@ -79,16 +79,16 @@
     <t xml:space="preserve">estender visualização de disponibilidade reserva para também locação</t>
   </si>
   <si>
+    <t xml:space="preserve">estender visualização de acompanhamento para também locação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar veículos com locação em progresso por filial/cliente pela filial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalizar locação</t>
+  </si>
+  <si>
     <t xml:space="preserve">Em Curso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estender visualização acompanhamento reserva para também locação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Listar veículos com locação em progresso por filial/cliente pela filial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalizar locação</t>
   </si>
   <si>
     <t xml:space="preserve">Manutenção</t>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t xml:space="preserve">Outro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Busca por busca aprimorada a genericidade </t>
   </si>
   <si>
     <t xml:space="preserve">arquivo de configurações</t>
@@ -674,24 +677,24 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -787,7 +790,6 @@
         <family val="0"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -858,10 +860,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ163"/>
+  <dimension ref="A1:AMJ164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -923,12 +925,12 @@
       <c r="C3" s="9"/>
       <c r="D3" s="10" t="n">
         <f aca="false">SUM(D6:D29)</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="n">
         <f aca="false">SUM(F6:F29)</f>
-        <v>44.99</v>
+        <v>48.99</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="0"/>
@@ -1172,13 +1174,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="22"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="30" t="n">
-        <v>0.536805555555556</v>
-      </c>
+      <c r="F12" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="29"/>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="K12" s="0"/>
@@ -1195,13 +1197,13 @@
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="29" t="s">
-        <v>19</v>
+      <c r="G13" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="28"/>
@@ -1222,51 +1224,49 @@
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="29" t="s">
-        <v>19</v>
+      <c r="G14" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H14" s="0"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
       <c r="K14" s="0"/>
       <c r="L14" s="0"/>
       <c r="M14" s="0"/>
       <c r="N14" s="0"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
-      <c r="C15" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="21" t="n">
-        <v>10</v>
-      </c>
+      <c r="C15" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="F15" s="21"/>
-      <c r="G15" s="29" t="s">
-        <v>19</v>
+      <c r="G15" s="33" t="s">
+        <v>22</v>
       </c>
       <c r="H15" s="0"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
       <c r="K15" s="0"/>
       <c r="L15" s="0"/>
       <c r="M15" s="0"/>
       <c r="N15" s="0"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
@@ -1287,8 +1287,8 @@
         <v>25</v>
       </c>
       <c r="H16" s="0"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
       <c r="K16" s="0"/>
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
@@ -1496,8 +1496,8 @@
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
-      <c r="L24" s="29" t="s">
-        <v>19</v>
+      <c r="L24" s="33" t="s">
+        <v>22</v>
       </c>
       <c r="M24" s="38" t="s">
         <v>38</v>
@@ -1866,17 +1866,21 @@
     </row>
     <row r="40" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="18"/>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="21"/>
+      <c r="D40" s="21" t="n">
+        <v>4</v>
+      </c>
       <c r="E40" s="22"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="35" t="s">
-        <v>25</v>
+      <c r="F40" s="21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G40" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H40" s="0"/>
       <c r="I40" s="0"/>
@@ -1890,7 +1894,7 @@
     </row>
     <row r="41" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="18"/>
-      <c r="B41" s="34"/>
+      <c r="B41" s="44"/>
       <c r="C41" s="41" t="s">
         <v>63</v>
       </c>
@@ -1910,14 +1914,18 @@
       <c r="AMI41" s="0"/>
       <c r="AMJ41" s="0"/>
     </row>
-    <row r="42" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="46"/>
-      <c r="B42" s="0"/>
-      <c r="C42" s="0"/>
-      <c r="D42" s="0"/>
-      <c r="E42" s="0"/>
-      <c r="F42" s="0"/>
-      <c r="G42" s="0"/>
+    <row r="42" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="18"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="35" t="s">
+        <v>25</v>
+      </c>
       <c r="H42" s="0"/>
       <c r="I42" s="0"/>
       <c r="J42" s="0"/>
@@ -2000,7 +2008,7 @@
       <c r="AMI46" s="0"/>
       <c r="AMJ46" s="0"/>
     </row>
-    <row r="47" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="46"/>
       <c r="B47" s="0"/>
       <c r="C47" s="0"/>
@@ -2090,9 +2098,13 @@
       <c r="AMI51" s="0"/>
       <c r="AMJ51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" s="48" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="46"/>
+      <c r="B52" s="0"/>
       <c r="C52" s="0"/>
+      <c r="D52" s="0"/>
+      <c r="E52" s="0"/>
+      <c r="F52" s="0"/>
       <c r="G52" s="0"/>
       <c r="H52" s="0"/>
       <c r="I52" s="0"/>
@@ -2100,6 +2112,9 @@
       <c r="K52" s="0"/>
       <c r="L52" s="0"/>
       <c r="M52" s="0"/>
+      <c r="N52" s="0"/>
+      <c r="AMI52" s="0"/>
+      <c r="AMJ52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="46"/>
@@ -2310,13 +2325,9 @@
       <c r="L71" s="0"/>
       <c r="M71" s="0"/>
     </row>
-    <row r="72" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="46"/>
-      <c r="B72" s="0"/>
       <c r="C72" s="0"/>
-      <c r="D72" s="0"/>
-      <c r="E72" s="0"/>
-      <c r="F72" s="0"/>
       <c r="G72" s="0"/>
       <c r="H72" s="0"/>
       <c r="I72" s="0"/>
@@ -2324,9 +2335,6 @@
       <c r="K72" s="0"/>
       <c r="L72" s="0"/>
       <c r="M72" s="0"/>
-      <c r="N72" s="0"/>
-      <c r="AMI72" s="0"/>
-      <c r="AMJ72" s="0"/>
     </row>
     <row r="73" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="46"/>
@@ -2418,7 +2426,7 @@
       <c r="AMI77" s="0"/>
       <c r="AMJ77" s="0"/>
     </row>
-    <row r="78" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="46"/>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
@@ -2436,9 +2444,13 @@
       <c r="AMI78" s="0"/>
       <c r="AMJ78" s="0"/>
     </row>
-    <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="46"/>
+      <c r="B79" s="0"/>
       <c r="C79" s="0"/>
+      <c r="D79" s="0"/>
+      <c r="E79" s="0"/>
+      <c r="F79" s="0"/>
       <c r="G79" s="0"/>
       <c r="H79" s="0"/>
       <c r="I79" s="0"/>
@@ -2446,14 +2458,13 @@
       <c r="K79" s="0"/>
       <c r="L79" s="0"/>
       <c r="M79" s="0"/>
-    </row>
-    <row r="80" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N79" s="0"/>
+      <c r="AMI79" s="0"/>
+      <c r="AMJ79" s="0"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="46"/>
-      <c r="B80" s="0"/>
       <c r="C80" s="0"/>
-      <c r="D80" s="0"/>
-      <c r="E80" s="0"/>
-      <c r="F80" s="0"/>
       <c r="G80" s="0"/>
       <c r="H80" s="0"/>
       <c r="I80" s="0"/>
@@ -2461,12 +2472,9 @@
       <c r="K80" s="0"/>
       <c r="L80" s="0"/>
       <c r="M80" s="0"/>
-      <c r="N80" s="0"/>
-      <c r="AMI80" s="0"/>
-      <c r="AMJ80" s="0"/>
     </row>
     <row r="81" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="48"/>
+      <c r="A81" s="46"/>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
       <c r="D81" s="0"/>
@@ -2645,9 +2653,13 @@
       <c r="AMI90" s="0"/>
       <c r="AMJ90" s="0"/>
     </row>
-    <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="48"/>
+      <c r="B91" s="0"/>
       <c r="C91" s="0"/>
+      <c r="D91" s="0"/>
+      <c r="E91" s="0"/>
+      <c r="F91" s="0"/>
       <c r="G91" s="0"/>
       <c r="H91" s="0"/>
       <c r="I91" s="0"/>
@@ -2655,14 +2667,13 @@
       <c r="K91" s="0"/>
       <c r="L91" s="0"/>
       <c r="M91" s="0"/>
-    </row>
-    <row r="92" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N91" s="0"/>
+      <c r="AMI91" s="0"/>
+      <c r="AMJ91" s="0"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="48"/>
-      <c r="B92" s="0"/>
       <c r="C92" s="0"/>
-      <c r="D92" s="0"/>
-      <c r="E92" s="0"/>
-      <c r="F92" s="0"/>
       <c r="G92" s="0"/>
       <c r="H92" s="0"/>
       <c r="I92" s="0"/>
@@ -2670,9 +2681,6 @@
       <c r="K92" s="0"/>
       <c r="L92" s="0"/>
       <c r="M92" s="0"/>
-      <c r="N92" s="0"/>
-      <c r="AMI92" s="0"/>
-      <c r="AMJ92" s="0"/>
     </row>
     <row r="93" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="48"/>
@@ -2728,9 +2736,13 @@
       <c r="AMI95" s="0"/>
       <c r="AMJ95" s="0"/>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="48"/>
+      <c r="B96" s="0"/>
       <c r="C96" s="0"/>
+      <c r="D96" s="0"/>
+      <c r="E96" s="0"/>
+      <c r="F96" s="0"/>
       <c r="G96" s="0"/>
       <c r="H96" s="0"/>
       <c r="I96" s="0"/>
@@ -2738,14 +2750,13 @@
       <c r="K96" s="0"/>
       <c r="L96" s="0"/>
       <c r="M96" s="0"/>
-    </row>
-    <row r="97" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N96" s="0"/>
+      <c r="AMI96" s="0"/>
+      <c r="AMJ96" s="0"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="48"/>
-      <c r="B97" s="0"/>
       <c r="C97" s="0"/>
-      <c r="D97" s="0"/>
-      <c r="E97" s="0"/>
-      <c r="F97" s="0"/>
       <c r="G97" s="0"/>
       <c r="H97" s="0"/>
       <c r="I97" s="0"/>
@@ -2753,12 +2764,9 @@
       <c r="K97" s="0"/>
       <c r="L97" s="0"/>
       <c r="M97" s="0"/>
-      <c r="N97" s="0"/>
-      <c r="AMI97" s="0"/>
-      <c r="AMJ97" s="0"/>
     </row>
     <row r="98" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="4"/>
+      <c r="A98" s="48"/>
       <c r="B98" s="0"/>
       <c r="C98" s="0"/>
       <c r="D98" s="0"/>
@@ -2829,8 +2837,13 @@
       <c r="AMI101" s="0"/>
       <c r="AMJ101" s="0"/>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="4"/>
+      <c r="B102" s="0"/>
       <c r="C102" s="0"/>
+      <c r="D102" s="0"/>
+      <c r="E102" s="0"/>
+      <c r="F102" s="0"/>
       <c r="G102" s="0"/>
       <c r="H102" s="0"/>
       <c r="I102" s="0"/>
@@ -2838,8 +2851,11 @@
       <c r="K102" s="0"/>
       <c r="L102" s="0"/>
       <c r="M102" s="0"/>
-    </row>
-    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="N102" s="0"/>
+      <c r="AMI102" s="0"/>
+      <c r="AMJ102" s="0"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="0"/>
       <c r="G103" s="0"/>
       <c r="H103" s="0"/>
@@ -3448,6 +3464,16 @@
       <c r="K163" s="0"/>
       <c r="L163" s="0"/>
       <c r="M163" s="0"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C164" s="0"/>
+      <c r="G164" s="0"/>
+      <c r="H164" s="0"/>
+      <c r="I164" s="0"/>
+      <c r="J164" s="0"/>
+      <c r="K164" s="0"/>
+      <c r="L164" s="0"/>
+      <c r="M164" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -3468,19 +3494,19 @@
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B40:B42"/>
   </mergeCells>
-  <conditionalFormatting sqref="C40:C41 C26:C38 C6:C24">
+  <conditionalFormatting sqref="C41:C42 C26:C38 C6:C24">
     <cfRule type="notContainsText" priority="2" operator="notContains" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="BLI" dxfId="0">
       <formula>ISERROR(SEARCH("BLI",C6))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22:L24 G6:G41">
+  <conditionalFormatting sqref="L22:L24 G6:G42">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("TRUE",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40:G41 G20:G29 G34:G35">
+  <conditionalFormatting sqref="G41:G42 G20:G29 G34:G35">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Pending" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("Pending",G20)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
backup obrigatório em tela'
</commit_message>
<xml_diff>
--- a/doc/Planejamento.xlsx
+++ b/doc/Planejamento.xlsx
@@ -862,8 +862,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ164"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1667,8 +1667,8 @@
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
       <c r="F31" s="21"/>
-      <c r="G31" s="34" t="s">
-        <v>24</v>
+      <c r="G31" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
@@ -1901,8 +1901,8 @@
       <c r="D41" s="21"/>
       <c r="E41" s="22"/>
       <c r="F41" s="21"/>
-      <c r="G41" s="34" t="s">
-        <v>24</v>
+      <c r="G41" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H41" s="0"/>
       <c r="I41" s="0"/>
@@ -3506,7 +3506,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G41:G42 G20:G29 G34:G35">
+  <conditionalFormatting sqref="G42 G20:G29 G34:G35">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Pending" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("Pending",G20)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
relatórios em tela completo
</commit_message>
<xml_diff>
--- a/doc/Planejamento.xlsx
+++ b/doc/Planejamento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
   <si>
     <t xml:space="preserve">Planejado</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">Listar veículos pendentes  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendente</t>
   </si>
   <si>
     <t xml:space="preserve">Listar veículos em manutenção
@@ -113,6 +110,9 @@
     <t xml:space="preserve">Histórico de manutenção por veículo</t>
   </si>
   <si>
+    <t xml:space="preserve">Em Curso</t>
+  </si>
+  <si>
     <t xml:space="preserve">clientes por tipo físico / jurídico</t>
   </si>
   <si>
@@ -128,15 +128,15 @@
     <t xml:space="preserve">locação por período</t>
   </si>
   <si>
+    <t xml:space="preserve">Pendente</t>
+  </si>
+  <si>
     <t xml:space="preserve">20 min = 0,33</t>
   </si>
   <si>
     <t xml:space="preserve">locação por cliente</t>
   </si>
   <si>
-    <t xml:space="preserve">Em Curso</t>
-  </si>
-  <si>
     <t xml:space="preserve">30 min = 0,50</t>
   </si>
   <si>
@@ -168,21 +168,6 @@
   </si>
   <si>
     <t xml:space="preserve">criação de tela para visualização de log por período para adms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cadastro simplificado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cliente físico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cliente jurídico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automóvel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caminhonete carga</t>
   </si>
   <si>
     <t xml:space="preserve">Backup</t>
@@ -438,14 +423,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -697,14 +682,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -713,16 +698,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -863,10 +848,10 @@
   <dimension ref="A1:AMJ164"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
@@ -1283,8 +1268,8 @@
       <c r="D16" s="21"/>
       <c r="E16" s="22"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="34" t="s">
-        <v>24</v>
+      <c r="G16" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H16" s="0"/>
       <c r="I16" s="30"/>
@@ -1305,13 +1290,13 @@
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="21"/>
-      <c r="G17" s="34" t="s">
-        <v>24</v>
+      <c r="G17" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
@@ -1329,13 +1314,13 @@
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="22"/>
       <c r="F18" s="21"/>
-      <c r="G18" s="34" t="s">
-        <v>24</v>
+      <c r="G18" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
@@ -1349,16 +1334,16 @@
         <v>10</v>
       </c>
       <c r="B19" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>27</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>28</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="22"/>
       <c r="F19" s="21"/>
-      <c r="G19" s="34" t="s">
-        <v>24</v>
+      <c r="G19" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
@@ -1373,13 +1358,13 @@
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22"/>
       <c r="F20" s="21"/>
-      <c r="G20" s="34" t="s">
-        <v>24</v>
+      <c r="G20" s="35" t="s">
+        <v>29</v>
       </c>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
@@ -1402,8 +1387,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F21" s="21"/>
-      <c r="G21" s="34" t="s">
-        <v>24</v>
+      <c r="G21" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
@@ -1429,8 +1414,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F22" s="21"/>
-      <c r="G22" s="34" t="s">
-        <v>24</v>
+      <c r="G22" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
@@ -1458,18 +1443,18 @@
         <v>#VALUE!</v>
       </c>
       <c r="F23" s="21"/>
-      <c r="G23" s="34" t="s">
-        <v>24</v>
+      <c r="G23" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H23" s="0"/>
       <c r="I23" s="0"/>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
       <c r="L23" s="38" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="M23" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N23" s="37"/>
       <c r="AMI23" s="0"/>
@@ -1481,7 +1466,7 @@
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="22" t="e">
@@ -1489,15 +1474,15 @@
         <v>#VALUE!</v>
       </c>
       <c r="F24" s="21"/>
-      <c r="G24" s="34" t="s">
-        <v>24</v>
+      <c r="G24" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
-      <c r="L24" s="39" t="s">
-        <v>37</v>
+      <c r="L24" s="35" t="s">
+        <v>29</v>
       </c>
       <c r="M24" s="37" t="s">
         <v>38</v>
@@ -1509,7 +1494,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="33"/>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="39" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="21"/>
@@ -1518,8 +1503,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F25" s="21"/>
-      <c r="G25" s="34" t="s">
-        <v>24</v>
+      <c r="G25" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
@@ -1547,8 +1532,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F26" s="21"/>
-      <c r="G26" s="34" t="s">
-        <v>24</v>
+      <c r="G26" s="40" t="s">
+        <v>35</v>
       </c>
       <c r="H26" s="0"/>
       <c r="I26" s="0"/>
@@ -1573,8 +1558,8 @@
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="21"/>
-      <c r="G27" s="34" t="s">
-        <v>24</v>
+      <c r="G27" s="40" t="s">
+        <v>35</v>
       </c>
       <c r="H27" s="0"/>
       <c r="I27" s="0"/>
@@ -1597,8 +1582,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F28" s="21"/>
-      <c r="G28" s="34" t="s">
-        <v>24</v>
+      <c r="G28" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H28" s="0"/>
       <c r="I28" s="0"/>
@@ -1621,8 +1606,8 @@
         <v>#VALUE!</v>
       </c>
       <c r="F29" s="21"/>
-      <c r="G29" s="34" t="s">
-        <v>24</v>
+      <c r="G29" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H29" s="0"/>
       <c r="I29" s="0"/>
@@ -1645,8 +1630,8 @@
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
       <c r="F30" s="21"/>
-      <c r="G30" s="34" t="s">
-        <v>24</v>
+      <c r="G30" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H30" s="0"/>
       <c r="I30" s="0"/>
@@ -1691,8 +1676,8 @@
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
       <c r="F32" s="21"/>
-      <c r="G32" s="34" t="s">
-        <v>24</v>
+      <c r="G32" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H32" s="0"/>
       <c r="I32" s="0"/>
@@ -1713,8 +1698,8 @@
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
       <c r="F33" s="21"/>
-      <c r="G33" s="34" t="s">
-        <v>24</v>
+      <c r="G33" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
@@ -1728,15 +1713,17 @@
     </row>
     <row r="34" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="41" t="s">
+      <c r="B34" s="33" t="s">
         <v>52</v>
+      </c>
+      <c r="C34" s="43" t="s">
+        <v>53</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
       <c r="F34" s="21"/>
-      <c r="G34" s="34" t="s">
-        <v>24</v>
+      <c r="G34" s="40" t="s">
+        <v>35</v>
       </c>
       <c r="H34" s="0"/>
       <c r="I34" s="0"/>
@@ -1750,15 +1737,17 @@
     </row>
     <row r="35" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="43" t="s">
-        <v>53</v>
+      <c r="B35" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="45" t="s">
+        <v>55</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="21"/>
-      <c r="G35" s="34" t="s">
-        <v>24</v>
+      <c r="G35" s="40" t="s">
+        <v>35</v>
       </c>
       <c r="H35" s="0"/>
       <c r="I35" s="0"/>
@@ -1772,17 +1761,21 @@
     </row>
     <row r="36" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
-      <c r="B36" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="21"/>
+      <c r="B36" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="21" t="n">
+        <v>4</v>
+      </c>
       <c r="E36" s="22"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="34" t="s">
-        <v>24</v>
+      <c r="F36" s="21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H36" s="0"/>
       <c r="I36" s="0"/>
@@ -1796,15 +1789,15 @@
     </row>
     <row r="37" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
-      <c r="B37" s="33"/>
+      <c r="B37" s="44"/>
       <c r="C37" s="41" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
       <c r="F37" s="21"/>
-      <c r="G37" s="34" t="s">
-        <v>24</v>
+      <c r="G37" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H37" s="0"/>
       <c r="I37" s="0"/>
@@ -1818,17 +1811,15 @@
     </row>
     <row r="38" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
-      <c r="B38" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="43" t="s">
-        <v>58</v>
+      <c r="B38" s="44"/>
+      <c r="C38" s="41" t="s">
+        <v>59</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
       <c r="F38" s="21"/>
-      <c r="G38" s="34" t="s">
-        <v>24</v>
+      <c r="G38" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="H38" s="0"/>
       <c r="I38" s="0"/>
@@ -1841,19 +1832,13 @@
       <c r="AMJ38" s="0"/>
     </row>
     <row r="39" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="18"/>
-      <c r="B39" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="34" t="s">
-        <v>24</v>
-      </c>
+      <c r="A39" s="46"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
       <c r="H39" s="0"/>
       <c r="I39" s="0"/>
       <c r="J39" s="0"/>
@@ -1865,23 +1850,13 @@
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="18"/>
-      <c r="B40" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="21" t="n">
-        <v>4</v>
-      </c>
-      <c r="E40" s="22"/>
-      <c r="F40" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="G40" s="23" t="s">
-        <v>11</v>
-      </c>
+      <c r="A40" s="46"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="G40" s="0"/>
       <c r="H40" s="0"/>
       <c r="I40" s="0"/>
       <c r="J40" s="0"/>
@@ -1893,17 +1868,13 @@
       <c r="AMJ40" s="0"/>
     </row>
     <row r="41" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="18"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="23" t="s">
-        <v>11</v>
-      </c>
+      <c r="A41" s="46"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="G41" s="0"/>
       <c r="H41" s="0"/>
       <c r="I41" s="0"/>
       <c r="J41" s="0"/>
@@ -1915,17 +1886,13 @@
       <c r="AMJ41" s="0"/>
     </row>
     <row r="42" s="2" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="18"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="34" t="s">
-        <v>24</v>
-      </c>
+      <c r="A42" s="46"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
       <c r="H42" s="0"/>
       <c r="I42" s="0"/>
       <c r="J42" s="0"/>
@@ -2409,7 +2376,7 @@
       <c r="AMJ76" s="0"/>
     </row>
     <row r="77" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="46"/>
+      <c r="A77" s="48"/>
       <c r="B77" s="0"/>
       <c r="C77" s="0"/>
       <c r="D77" s="0"/>
@@ -2427,7 +2394,7 @@
       <c r="AMJ77" s="0"/>
     </row>
     <row r="78" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="46"/>
+      <c r="A78" s="48"/>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
       <c r="D78" s="0"/>
@@ -2445,7 +2412,7 @@
       <c r="AMJ78" s="0"/>
     </row>
     <row r="79" s="2" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="46"/>
+      <c r="A79" s="48"/>
       <c r="B79" s="0"/>
       <c r="C79" s="0"/>
       <c r="D79" s="0"/>
@@ -2463,7 +2430,7 @@
       <c r="AMJ79" s="0"/>
     </row>
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="46"/>
+      <c r="A80" s="48"/>
       <c r="C80" s="0"/>
       <c r="G80" s="0"/>
       <c r="H80" s="0"/>
@@ -2474,7 +2441,7 @@
       <c r="M80" s="0"/>
     </row>
     <row r="81" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="46"/>
+      <c r="A81" s="48"/>
       <c r="B81" s="0"/>
       <c r="C81" s="0"/>
       <c r="D81" s="0"/>
@@ -2701,7 +2668,7 @@
       <c r="AMJ93" s="0"/>
     </row>
     <row r="94" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="48"/>
+      <c r="A94" s="4"/>
       <c r="B94" s="0"/>
       <c r="C94" s="0"/>
       <c r="D94" s="0"/>
@@ -2719,7 +2686,7 @@
       <c r="AMJ94" s="0"/>
     </row>
     <row r="95" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="48"/>
+      <c r="A95" s="4"/>
       <c r="B95" s="0"/>
       <c r="C95" s="0"/>
       <c r="D95" s="0"/>
@@ -2737,7 +2704,7 @@
       <c r="AMJ95" s="0"/>
     </row>
     <row r="96" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="48"/>
+      <c r="A96" s="4"/>
       <c r="B96" s="0"/>
       <c r="C96" s="0"/>
       <c r="D96" s="0"/>
@@ -2755,7 +2722,7 @@
       <c r="AMJ96" s="0"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="48"/>
+      <c r="A97" s="4"/>
       <c r="C97" s="0"/>
       <c r="G97" s="0"/>
       <c r="H97" s="0"/>
@@ -2766,7 +2733,7 @@
       <c r="M97" s="0"/>
     </row>
     <row r="98" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="48"/>
+      <c r="A98" s="0"/>
       <c r="B98" s="0"/>
       <c r="C98" s="0"/>
       <c r="D98" s="0"/>
@@ -2784,7 +2751,7 @@
       <c r="AMJ98" s="0"/>
     </row>
     <row r="99" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="4"/>
+      <c r="A99" s="0"/>
       <c r="B99" s="0"/>
       <c r="C99" s="0"/>
       <c r="D99" s="0"/>
@@ -2802,7 +2769,7 @@
       <c r="AMJ99" s="0"/>
     </row>
     <row r="100" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="4"/>
+      <c r="A100" s="0"/>
       <c r="B100" s="0"/>
       <c r="C100" s="0"/>
       <c r="D100" s="0"/>
@@ -2820,7 +2787,7 @@
       <c r="AMJ100" s="0"/>
     </row>
     <row r="101" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="4"/>
+      <c r="A101" s="0"/>
       <c r="B101" s="0"/>
       <c r="C101" s="0"/>
       <c r="D101" s="0"/>
@@ -2838,7 +2805,7 @@
       <c r="AMJ101" s="0"/>
     </row>
     <row r="102" s="2" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="4"/>
+      <c r="A102" s="0"/>
       <c r="B102" s="0"/>
       <c r="C102" s="0"/>
       <c r="D102" s="0"/>
@@ -3436,8 +3403,6 @@
       <c r="M160" s="0"/>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C161" s="0"/>
-      <c r="G161" s="0"/>
       <c r="H161" s="0"/>
       <c r="I161" s="0"/>
       <c r="J161" s="0"/>
@@ -3446,8 +3411,6 @@
       <c r="M161" s="0"/>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C162" s="0"/>
-      <c r="G162" s="0"/>
       <c r="H162" s="0"/>
       <c r="I162" s="0"/>
       <c r="J162" s="0"/>
@@ -3456,8 +3419,6 @@
       <c r="M162" s="0"/>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C163" s="0"/>
-      <c r="G163" s="0"/>
       <c r="H163" s="0"/>
       <c r="I163" s="0"/>
       <c r="J163" s="0"/>
@@ -3466,8 +3427,6 @@
       <c r="M163" s="0"/>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C164" s="0"/>
-      <c r="G164" s="0"/>
       <c r="H164" s="0"/>
       <c r="I164" s="0"/>
       <c r="J164" s="0"/>
@@ -3476,7 +3435,7 @@
       <c r="M164" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="17">
     <mergeCell ref="B1:N1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -3492,26 +3451,25 @@
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="M26:N26"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B36:B38"/>
   </mergeCells>
-  <conditionalFormatting sqref="C41:C42 C26:C38 C6:C24">
+  <conditionalFormatting sqref="C37:C38 C26:C34 C6:C24">
     <cfRule type="notContainsText" priority="2" operator="notContains" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="BLI" dxfId="0">
       <formula>ISERROR(SEARCH("BLI",C6))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22:L24 G6:G42">
+  <conditionalFormatting sqref="L22:L24 G6:G38">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("TRUE",G6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G42 G20:G29 G34:G35">
+  <conditionalFormatting sqref="G26:G27">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Pending" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("Pending",G20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pending",G26)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Done" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("Done",G20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",G26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>